<commit_message>
First attempt at implementing DEs
</commit_message>
<xml_diff>
--- a/MATLAB Code/config.xlsx
+++ b/MATLAB Code/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ikeni\Desktop\Optimal Estimation\USU_Optimal_Estimation_Project\MATLAB Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140AC9FC-9BD3-493F-B112-2EC6B25B26A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A9FCBF-4E5C-4F1D-A3CE-3961172A38D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-165" windowWidth="20520" windowHeight="13245" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="894" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="198">
   <si>
     <t>Value</t>
   </si>
@@ -454,9 +454,6 @@
     <t>z component of position of ground coil(inertial)</t>
   </si>
   <si>
-    <t>ang_rate</t>
-  </si>
-  <si>
     <t>st_angle</t>
   </si>
   <si>
@@ -589,21 +586,73 @@
     <t>tau_g</t>
   </si>
   <si>
-    <t>accelerometer time constant</t>
-  </si>
-  <si>
-    <t>gyroscope time constant</t>
+    <t>accelerometer ECRV time constant</t>
+  </si>
+  <si>
+    <t>gyroscope ECRV time constant</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>MHz</t>
+  </si>
+  <si>
+    <t>Carrier frequency of ground circuit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c </t>
+  </si>
+  <si>
+    <t>Speed of light in air</t>
+  </si>
+  <si>
+    <t>r2_z</t>
+  </si>
+  <si>
+    <t>r2_y</t>
+  </si>
+  <si>
+    <t>r2_x</t>
+  </si>
+  <si>
+    <t>r1_z</t>
+  </si>
+  <si>
+    <t>r1_y</t>
+  </si>
+  <si>
+    <t>r1_x</t>
+  </si>
+  <si>
+    <t>x component of sensing coil 1 position wrt to body frame</t>
+  </si>
+  <si>
+    <t>y component of sensing coil 1 position wrt to body frame</t>
+  </si>
+  <si>
+    <t>z component of sensing coil 1 position wrt to body frame</t>
+  </si>
+  <si>
+    <t>x component of sensing coil 2 position wrt to body frame</t>
+  </si>
+  <si>
+    <t>y component of sensing coil 2 position wrt to body frame</t>
+  </si>
+  <si>
+    <t>z component of sensing coil 2 position wrt to body frame</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.00000000E+00"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0000000"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -642,7 +691,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -792,13 +841,117 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color theme="0" tint="-0.14999847407452621"/>
       </left>
       <right style="thin">
         <color theme="0" tint="-0.14999847407452621"/>
       </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -806,7 +959,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -872,7 +1025,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1213,14 +1379,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="39.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="75.59765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
@@ -1249,7 +1415,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="54">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="C2" s="53" t="s">
         <v>5</v>
@@ -1259,7 +1425,7 @@
       </c>
       <c r="E2" s="55">
         <f t="shared" ref="E2:E7" si="0">B2</f>
-        <v>2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="53" customFormat="1" x14ac:dyDescent="0.45">
@@ -1267,7 +1433,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="54">
-        <v>0.25</v>
+        <v>0.01</v>
       </c>
       <c r="C3" s="53" t="s">
         <v>5</v>
@@ -1277,7 +1443,7 @@
       </c>
       <c r="E3" s="55">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="53" customFormat="1" x14ac:dyDescent="0.45">
@@ -1303,7 +1469,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="56">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C5" s="53" t="s">
         <v>4</v>
@@ -1313,7 +1479,7 @@
       </c>
       <c r="E5" s="55">
         <f>B5</f>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="53" customFormat="1" x14ac:dyDescent="0.45">
@@ -1390,7 +1556,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" s="53" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="73" t="s">
         <v>40</v>
       </c>
       <c r="B10" s="56">
@@ -1408,17 +1574,17 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="65" t="s">
-        <v>175</v>
+      <c r="A11" s="74" t="s">
+        <v>174</v>
       </c>
       <c r="B11" s="2">
         <v>2</v>
       </c>
-      <c r="C11" s="65" t="s">
+      <c r="C11" s="53" t="s">
+        <v>175</v>
+      </c>
+      <c r="D11" s="53" t="s">
         <v>176</v>
-      </c>
-      <c r="D11" s="65" t="s">
-        <v>177</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="1"/>
@@ -1426,17 +1592,17 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="65" t="s">
-        <v>178</v>
+      <c r="A12" s="53" t="s">
+        <v>177</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="C12" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="65" t="s">
-        <v>180</v>
+      <c r="D12" s="53" t="s">
+        <v>179</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="1"/>
@@ -1444,24 +1610,171 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="65" t="s">
-        <v>179</v>
+      <c r="A13" s="53" t="s">
+        <v>178</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
       </c>
-      <c r="C13" s="65" t="s">
+      <c r="C13" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="65" t="s">
-        <v>181</v>
+      <c r="D13" s="53" t="s">
+        <v>180</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" s="53" t="s">
+        <v>181</v>
+      </c>
+      <c r="B14" s="2">
+        <v>122</v>
+      </c>
+      <c r="C14" s="53" t="s">
+        <v>182</v>
+      </c>
+      <c r="D14" s="53" t="s">
+        <v>183</v>
+      </c>
+      <c r="E14" s="1">
+        <f>B14*1000000</f>
+        <v>122000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" s="53" t="s">
+        <v>184</v>
+      </c>
+      <c r="B15" s="2">
+        <v>299702547</v>
+      </c>
+      <c r="C15" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" s="53" t="s">
+        <v>185</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" ref="E15:E21" si="2">B15</f>
+        <v>299702547</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" s="53" t="s">
+        <v>191</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C16" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="76" t="s">
+        <v>192</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" s="53" t="s">
+        <v>190</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="76" t="s">
+        <v>193</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" s="53" t="s">
+        <v>189</v>
+      </c>
+      <c r="B18" s="75">
+        <v>0</v>
+      </c>
+      <c r="C18" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="76" t="s">
+        <v>194</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" s="53" t="s">
+        <v>188</v>
+      </c>
+      <c r="B19" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="C19" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="76" t="s">
+        <v>195</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" s="53" t="s">
+        <v>187</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="76" t="s">
+        <v>196</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" s="53" t="s">
+        <v>186</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
+      <c r="C21" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="76" t="s">
+        <v>197</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" s="76"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="C26" s="49"/>
     </row>
   </sheetData>
@@ -1533,8 +1846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D12A37-CB3D-4FDB-95C9-F32EFDA07C44}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1621,7 +1934,7 @@
         <v>53</v>
       </c>
       <c r="B5" s="34">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="C5" s="38" t="s">
         <v>120</v>
@@ -1631,7 +1944,7 @@
       </c>
       <c r="E5" s="32">
         <f>B5</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
@@ -1639,7 +1952,7 @@
         <v>54</v>
       </c>
       <c r="B6" s="34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="38" t="s">
         <v>120</v>
@@ -1649,7 +1962,7 @@
       </c>
       <c r="E6" s="32">
         <f t="shared" ref="E6:E7" si="1">B6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
@@ -1674,7 +1987,7 @@
       <c r="A8" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="77">
         <v>1</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -1684,6 +1997,7 @@
         <v>125</v>
       </c>
       <c r="E8" s="12">
+        <f>B8</f>
         <v>1</v>
       </c>
     </row>
@@ -1700,7 +2014,8 @@
       <c r="D9" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
+        <f t="shared" ref="E9:E11" si="2">B9</f>
         <v>0</v>
       </c>
     </row>
@@ -1717,7 +2032,8 @@
       <c r="D10" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1725,7 +2041,7 @@
       <c r="A11" s="58" t="s">
         <v>124</v>
       </c>
-      <c r="B11" s="46">
+      <c r="B11" s="78">
         <v>0</v>
       </c>
       <c r="C11" s="8" t="s">
@@ -1734,22 +2050,23 @@
       <c r="D11" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="12">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B12" s="4">
         <v>0</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>171</v>
       </c>
       <c r="E12" s="61">
         <f>RADIANS(B12)</f>
@@ -1758,16 +2075,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="63" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B13" s="57">
         <v>0</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E13" s="43">
         <f>RADIANS(B13)</f>
@@ -1776,16 +2093,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="64" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B14" s="8">
         <v>0</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E14" s="44">
         <f>RADIANS(B14)</f>
@@ -1794,16 +2111,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="62" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B15" s="4">
         <v>0</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E15" s="61">
         <f>RADIANS(B15)</f>
@@ -1812,16 +2129,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="62" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B16" s="4">
         <v>0</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E16" s="61">
         <f>B16*g2mps2</f>
@@ -1830,16 +2147,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="63" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B17" s="16">
         <v>0</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E17" s="43">
         <f>B17*g2mps2</f>
@@ -1848,16 +2165,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="64" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B18" s="8">
         <v>0</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E18" s="44">
         <f>B18*g2mps2</f>
@@ -1866,7 +2183,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="63" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B19" s="6">
         <v>0</v>
@@ -1875,7 +2192,7 @@
         <v>24</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E19" s="43">
         <f>RADIANS(B19)/hr2sec</f>
@@ -1884,7 +2201,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="63" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B20" s="16">
         <v>0</v>
@@ -1893,7 +2210,7 @@
         <v>24</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E20" s="43">
         <f>RADIANS(B20)/hr2sec</f>
@@ -1902,7 +2219,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="64" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B21" s="8">
         <v>0</v>
@@ -1911,7 +2228,7 @@
         <v>24</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E21" s="44">
         <f>RADIANS(B21)/hr2sec</f>
@@ -1941,7 +2258,7 @@
         <v>130</v>
       </c>
       <c r="B23" s="57">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>8</v>
@@ -1950,8 +2267,8 @@
         <v>133</v>
       </c>
       <c r="E23" s="59">
-        <f t="shared" ref="E23:E24" si="2">B23</f>
-        <v>1</v>
+        <f t="shared" ref="E23:E24" si="3">B23</f>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
@@ -1968,7 +2285,7 @@
         <v>134</v>
       </c>
       <c r="E24" s="60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2029,7 +2346,7 @@
         <v>m</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E2" s="61">
         <f t="shared" ref="E2:E7" si="0">B2</f>
@@ -2049,7 +2366,7 @@
         <v>m</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E3" s="43">
         <f t="shared" si="0"/>
@@ -2069,7 +2386,7 @@
         <v>m</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E4" s="43">
         <f t="shared" si="0"/>
@@ -2089,7 +2406,7 @@
         <v>m/sec</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E5" s="43">
         <f t="shared" si="0"/>
@@ -2109,7 +2426,7 @@
         <v>m/sec</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E6" s="43">
         <f t="shared" si="0"/>
@@ -2129,7 +2446,7 @@
         <v>m/sec</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E7" s="43">
         <f t="shared" si="0"/>
@@ -2139,7 +2456,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B8" s="6">
         <v>0.01</v>
@@ -2148,7 +2465,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E8" s="43">
         <f>B8</f>
@@ -2158,7 +2475,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" s="6">
         <v>0.02</v>
@@ -2167,7 +2484,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E9" s="43">
         <f t="shared" ref="E9:E10" si="1">B9</f>
@@ -2177,7 +2494,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B10" s="6">
         <v>0.03</v>
@@ -2186,7 +2503,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E10" s="43">
         <f t="shared" si="1"/>
@@ -2196,16 +2513,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B11" s="16">
         <v>1E-3</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E11" s="43">
         <f>B11*g2mps2</f>
@@ -2215,16 +2532,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B12" s="16">
         <v>2E-3</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E12" s="43">
         <f>B12*g2mps2</f>
@@ -2234,16 +2551,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B13" s="16">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E13" s="43">
         <f>B13*g2mps2</f>
@@ -2311,7 +2628,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B17" s="6">
         <v>0.11</v>
@@ -2320,7 +2637,7 @@
         <v>8</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E17" s="43">
         <f t="shared" ref="E17:E19" si="2">B17</f>
@@ -2329,7 +2646,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B18" s="6">
         <v>0.22</v>
@@ -2338,7 +2655,7 @@
         <v>8</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E18" s="43">
         <f t="shared" si="2"/>
@@ -2347,7 +2664,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B19" s="8">
         <v>0.33</v>
@@ -2356,7 +2673,7 @@
         <v>8</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E19" s="44">
         <f t="shared" si="2"/>
@@ -2371,10 +2688,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C720B3-BEEA-4D2E-BE7C-7EC9578AFA75}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2384,7 +2701,7 @@
     <col min="5" max="5" width="14.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -2402,180 +2719,163 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="A2" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="66">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="66">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="66">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="67">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="A3" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="6">
         <v>4</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="6">
         <v>6</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="6">
         <v>4</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="69">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="71">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="71">
         <v>10</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="71">
         <v>7</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="72">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="A5" s="65" t="s">
         <v>135</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="66">
         <v>11</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="66">
+        <v>11</v>
+      </c>
+      <c r="D5" s="66">
+        <v>10</v>
+      </c>
+      <c r="E5" s="67">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" s="68" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" s="6">
+        <v>12</v>
+      </c>
+      <c r="C6" s="6">
+        <v>14</v>
+      </c>
+      <c r="D6" s="6">
+        <v>11</v>
+      </c>
+      <c r="E6" s="69">
         <v>13</v>
       </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>136</v>
-      </c>
-      <c r="B6">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" s="68" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="6">
+        <v>15</v>
+      </c>
+      <c r="C7" s="6">
+        <v>17</v>
+      </c>
+      <c r="D7" s="6">
         <v>14</v>
       </c>
-      <c r="C6">
-        <v>14</v>
-      </c>
-      <c r="D6">
-        <v>13</v>
-      </c>
-      <c r="E6">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="E7" s="69">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="70" t="s">
         <v>137</v>
       </c>
-      <c r="B7">
-        <v>15</v>
-      </c>
-      <c r="C7">
+      <c r="B8" s="71">
+        <v>18</v>
+      </c>
+      <c r="C8" s="71">
+        <v>20</v>
+      </c>
+      <c r="D8" s="71">
         <v>17</v>
       </c>
-      <c r="D7">
-        <v>14</v>
-      </c>
-      <c r="E7">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8">
-        <v>18</v>
-      </c>
-      <c r="C8">
-        <v>20</v>
-      </c>
-      <c r="D8">
-        <v>17</v>
-      </c>
-      <c r="E8">
+      <c r="E8" s="72">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>138</v>
-      </c>
-      <c r="B9">
-        <v>21</v>
-      </c>
-      <c r="C9">
-        <v>23</v>
-      </c>
-      <c r="D9">
-        <v>20</v>
-      </c>
-      <c r="E9">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+      <c r="A9" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="B10">
+      <c r="B9" s="66">
         <f>B2</f>
         <v>1</v>
       </c>
-      <c r="C10">
-        <f>C6</f>
-        <v>14</v>
-      </c>
-      <c r="D10">
+      <c r="C9" s="66">
+        <f>C5</f>
+        <v>11</v>
+      </c>
+      <c r="D9" s="66">
         <v>1</v>
       </c>
-      <c r="E10">
-        <f>E6</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+      <c r="E9" s="67">
+        <f>E5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="B11">
-        <f>B5</f>
+      <c r="B10" s="71">
+        <f>B6</f>
+        <v>12</v>
+      </c>
+      <c r="C10" s="71">
+        <f>C8</f>
+        <v>20</v>
+      </c>
+      <c r="D10" s="71">
+        <f>D6</f>
         <v>11</v>
       </c>
-      <c r="C11">
-        <f>C9</f>
-        <v>23</v>
-      </c>
-      <c r="D11">
-        <f>D5</f>
-        <v>10</v>
-      </c>
-      <c r="E11">
-        <f>E9</f>
-        <v>22</v>
+      <c r="E10" s="72">
+        <f>E8</f>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2588,7 +2888,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2598,7 +2898,7 @@
     <col min="5" max="5" width="14.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -2616,145 +2916,145 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="A2" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="66">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="66">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="66">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="67">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="A3" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="6">
         <v>4</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="6">
         <v>6</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="6">
         <v>4</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="69">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="71">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="71">
         <v>10</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="71">
         <v>7</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="72">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="A5" s="65" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="66">
+        <v>11</v>
+      </c>
+      <c r="C5" s="66">
+        <v>13</v>
+      </c>
+      <c r="D5" s="66">
+        <v>10</v>
+      </c>
+      <c r="E5" s="67">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" s="68" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="6">
+        <v>14</v>
+      </c>
+      <c r="C6" s="6">
+        <v>16</v>
+      </c>
+      <c r="D6" s="6">
+        <v>13</v>
+      </c>
+      <c r="E6" s="69">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="70" t="s">
         <v>137</v>
       </c>
-      <c r="B5">
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <v>13</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6">
-        <v>14</v>
-      </c>
-      <c r="C6">
+      <c r="B7" s="71">
+        <v>17</v>
+      </c>
+      <c r="C7" s="71">
+        <v>19</v>
+      </c>
+      <c r="D7" s="71">
         <v>16</v>
       </c>
-      <c r="D6">
-        <v>13</v>
-      </c>
-      <c r="E6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>138</v>
-      </c>
-      <c r="B7">
-        <v>17</v>
-      </c>
-      <c r="C7">
-        <v>19</v>
-      </c>
-      <c r="D7">
-        <v>16</v>
-      </c>
-      <c r="E7">
+      <c r="E7" s="72">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="A8" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="66">
         <f>B2</f>
         <v>1</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="66">
         <f>C4</f>
         <v>10</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="66">
         <f>D2</f>
         <v>1</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="67">
         <f>E4</f>
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="71">
         <f>B5</f>
         <v>11</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="71">
         <f>C7</f>
         <v>19</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="71">
         <f>D5</f>
         <v>10</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="72">
         <f>E7</f>
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
linear error state modeling DONE
</commit_message>
<xml_diff>
--- a/MATLAB Code/config.xlsx
+++ b/MATLAB Code/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ikeni\Desktop\Optimal Estimation\USU_Optimal_Estimation_Project\MATLAB Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8EFA2E-2A01-4731-9569-3FF3FF0CD785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB4FE70-5AB3-48A6-8991-09701414A5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-195" windowWidth="20520" windowHeight="13275" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -1253,7 +1253,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1288,7 +1288,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="50">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
       <c r="C2" s="49" t="s">
         <v>5</v>
@@ -1298,7 +1298,7 @@
       </c>
       <c r="E2" s="51">
         <f t="shared" ref="E2:E7" si="0">B2</f>
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
@@ -1397,7 +1397,7 @@
         <v>38</v>
       </c>
       <c r="B8" s="52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="49" t="s">
         <v>4</v>
@@ -1407,7 +1407,7 @@
       </c>
       <c r="E8" s="51">
         <f t="shared" ref="E8:E13" si="1">B8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
@@ -1415,7 +1415,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="49" t="s">
         <v>4</v>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="E9" s="51">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
@@ -1735,7 +1735,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2070,8 +2070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A73" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Fixed some errors in the F matrix Fixed some NED vs. ENU errors Still having problems getting truth to match nav propagation
</commit_message>
<xml_diff>
--- a/MATLAB Code/config.xlsx
+++ b/MATLAB Code/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ikeni\Desktop\Optimal Estimation\USU_Optimal_Estimation_Project\MATLAB Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\student-repos\ifroisland\MATLAB Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB4FE70-5AB3-48A6-8991-09701414A5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055A28B3-8F27-48DC-916E-BE0D207A5244}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20715" windowHeight="13275" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -32,17 +32,6 @@
     <definedName name="min2sec">Constants!$B$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -1253,20 +1242,20 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
         <v>3</v>
       </c>
@@ -1283,12 +1272,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="50">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="C2" s="49" t="s">
         <v>5</v>
@@ -1298,10 +1287,10 @@
       </c>
       <c r="E2" s="51">
         <f t="shared" ref="E2:E7" si="0">B2</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
         <v>22</v>
       </c>
@@ -1319,7 +1308,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
         <v>44</v>
       </c>
@@ -1337,7 +1326,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
         <v>12</v>
       </c>
@@ -1355,7 +1344,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="49" t="s">
         <v>47</v>
       </c>
@@ -1373,7 +1362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="49" t="s">
         <v>92</v>
       </c>
@@ -1392,7 +1381,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="49" t="s">
         <v>38</v>
       </c>
@@ -1410,12 +1399,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="49" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="49" t="s">
         <v>4</v>
@@ -1425,10 +1414,10 @@
       </c>
       <c r="E9" s="51">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="61" t="s">
         <v>40</v>
       </c>
@@ -1446,7 +1435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>139</v>
       </c>
@@ -1464,7 +1453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="49" t="s">
         <v>142</v>
       </c>
@@ -1482,7 +1471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="49" t="s">
         <v>143</v>
       </c>
@@ -1500,7 +1489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="49" t="s">
         <v>146</v>
       </c>
@@ -1518,7 +1507,7 @@
         <v>122000000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="49" t="s">
         <v>149</v>
       </c>
@@ -1536,7 +1525,7 @@
         <v>299702547</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="49" t="s">
         <v>156</v>
       </c>
@@ -1554,7 +1543,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="49" t="s">
         <v>155</v>
       </c>
@@ -1572,7 +1561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="49" t="s">
         <v>154</v>
       </c>
@@ -1590,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="49" t="s">
         <v>153</v>
       </c>
@@ -1608,7 +1597,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="49" t="s">
         <v>152</v>
       </c>
@@ -1626,7 +1615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="49" t="s">
         <v>151</v>
       </c>
@@ -1644,7 +1633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="64" t="s">
         <v>132</v>
       </c>
@@ -1662,7 +1651,7 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C26" s="45"/>
     </row>
   </sheetData>
@@ -1679,12 +1668,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1692,7 +1681,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1700,7 +1689,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1709,7 +1698,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1717,7 +1706,7 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>107</v>
       </c>
@@ -1735,18 +1724,18 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
@@ -1763,7 +1752,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>174</v>
       </c>
@@ -1781,7 +1770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>173</v>
       </c>
@@ -1799,7 +1788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="65" t="s">
         <v>170</v>
       </c>
@@ -1815,7 +1804,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="65" t="s">
         <v>178</v>
       </c>
@@ -1831,7 +1820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="65" t="s">
         <v>115</v>
       </c>
@@ -1847,7 +1836,7 @@
         <v>8.7266462599716474E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
         <v>133</v>
       </c>
@@ -1865,7 +1854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="59" t="s">
         <v>135</v>
       </c>
@@ -1883,7 +1872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
         <v>136</v>
       </c>
@@ -1901,7 +1890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="59" t="s">
         <v>134</v>
       </c>
@@ -1919,7 +1908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="59" t="s">
         <v>137</v>
       </c>
@@ -1937,7 +1926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
         <v>138</v>
       </c>
@@ -1955,7 +1944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
         <v>109</v>
       </c>
@@ -1973,7 +1962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
         <v>110</v>
       </c>
@@ -1991,7 +1980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="54" t="s">
         <v>111</v>
       </c>
@@ -2009,55 +1998,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="E16" s="57"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="16"/>
       <c r="C17" s="6"/>
       <c r="E17" s="39"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="8"/>
       <c r="C18" s="17"/>
       <c r="E18" s="40"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="E19" s="39"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="16"/>
       <c r="C20" s="6"/>
       <c r="E20" s="39"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="E21" s="40"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="53"/>
       <c r="C22" s="16"/>
       <c r="E22" s="55"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="53"/>
       <c r="C23" s="16"/>
       <c r="E23" s="55"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="42"/>
       <c r="C24" s="17"/>
       <c r="E24" s="56"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D28" s="6"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="6"/>
     </row>
   </sheetData>
@@ -2070,19 +2059,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.59765625" customWidth="1"/>
-    <col min="5" max="5" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>3</v>
       </c>
@@ -2099,7 +2088,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>85</v>
       </c>
@@ -2119,7 +2108,7 @@
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>86</v>
       </c>
@@ -2139,7 +2128,7 @@
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>87</v>
       </c>
@@ -2159,7 +2148,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>88</v>
       </c>
@@ -2179,7 +2168,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>89</v>
       </c>
@@ -2199,7 +2188,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>90</v>
       </c>
@@ -2219,7 +2208,7 @@
       </c>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>129</v>
       </c>
@@ -2238,7 +2227,7 @@
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>130</v>
       </c>
@@ -2257,7 +2246,7 @@
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>131</v>
       </c>
@@ -2276,7 +2265,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>121</v>
       </c>
@@ -2295,7 +2284,7 @@
       </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>122</v>
       </c>
@@ -2314,7 +2303,7 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>123</v>
       </c>
@@ -2333,7 +2322,7 @@
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>26</v>
       </c>
@@ -2353,7 +2342,7 @@
       </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>28</v>
       </c>
@@ -2372,7 +2361,7 @@
         <v>9.6962736221907197E-6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>29</v>
       </c>
@@ -2391,7 +2380,7 @@
         <v>1.454441043328608E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>125</v>
       </c>
@@ -2409,7 +2398,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>126</v>
       </c>
@@ -2427,7 +2416,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>127</v>
       </c>
@@ -2459,14 +2448,14 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -2483,7 +2472,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>176</v>
       </c>
@@ -2500,7 +2489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>177</v>
       </c>
@@ -2517,7 +2506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>175</v>
       </c>
@@ -2534,7 +2523,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>178</v>
       </c>
@@ -2551,7 +2540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>115</v>
       </c>
@@ -2568,7 +2557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>116</v>
       </c>
@@ -2585,7 +2574,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>49</v>
       </c>
@@ -2602,7 +2591,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>117</v>
       </c>
@@ -2619,7 +2608,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
@@ -2639,7 +2628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>43</v>
       </c>
@@ -2673,14 +2662,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -2697,7 +2686,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -2714,7 +2703,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>31</v>
       </c>
@@ -2731,7 +2720,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
@@ -2748,7 +2737,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>116</v>
       </c>
@@ -2765,7 +2754,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>49</v>
       </c>
@@ -2782,7 +2771,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>117</v>
       </c>
@@ -2799,7 +2788,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>42</v>
       </c>
@@ -2820,7 +2809,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>43</v>
       </c>
@@ -2852,17 +2841,17 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.59765625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>3</v>
       </c>
@@ -2879,7 +2868,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>93</v>
       </c>
@@ -2898,7 +2887,7 @@
         <v>1.6000000000000003E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
@@ -2917,7 +2906,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -2935,7 +2924,7 @@
         <v>4.8481368110953598E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>71</v>
       </c>
@@ -2953,7 +2942,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>72</v>
       </c>
@@ -2971,7 +2960,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>73</v>
       </c>
@@ -2989,7 +2978,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>74</v>
       </c>
@@ -3007,7 +2996,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>75</v>
       </c>
@@ -3025,7 +3014,7 @@
         <v>1.4544410433286079E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="43" t="s">
         <v>97</v>
       </c>
@@ -3043,7 +3032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>98</v>
       </c>
@@ -3061,7 +3050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>101</v>
       </c>
@@ -3079,7 +3068,7 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>103</v>
       </c>
@@ -3097,7 +3086,7 @@
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>105</v>
       </c>
@@ -3129,17 +3118,17 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.73046875" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.3984375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1328125" style="6"/>
+    <col min="4" max="4" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
@@ -3156,7 +3145,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>55</v>
       </c>
@@ -3174,7 +3163,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>57</v>
       </c>
@@ -3192,7 +3181,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>58</v>
       </c>
@@ -3210,7 +3199,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>59</v>
       </c>
@@ -3228,7 +3217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>62</v>
       </c>
@@ -3246,7 +3235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>63</v>
       </c>
@@ -3264,7 +3253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>76</v>
       </c>
@@ -3282,7 +3271,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>77</v>
       </c>
@@ -3300,7 +3289,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>78</v>
       </c>
@@ -3318,7 +3307,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>82</v>
       </c>
@@ -3337,7 +3326,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>83</v>
       </c>
@@ -3356,7 +3345,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>84</v>
       </c>
@@ -3375,7 +3364,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>79</v>
       </c>
@@ -3394,7 +3383,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>80</v>
       </c>
@@ -3413,7 +3402,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>81</v>
       </c>
@@ -3432,7 +3421,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>67</v>
       </c>
@@ -3451,7 +3440,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>69</v>
       </c>
@@ -3470,7 +3459,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>70</v>
       </c>
@@ -3501,18 +3490,18 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.73046875" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.59765625" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.86328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.73046875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="14.3984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1328125" style="6"/>
+    <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>3</v>
       </c>
@@ -3529,7 +3518,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
         <f>truthStateParams!A2</f>
         <v>Q_grav</v>
@@ -3552,7 +3541,7 @@
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
         <f>truthStateParams!A3</f>
         <v>sig_gyro_ss</v>
@@ -3575,7 +3564,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="str">
         <f>truthStateParams!A4</f>
         <v>arw</v>
@@ -3598,7 +3587,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="str">
         <f>truthStateParams!A5</f>
         <v>sig_st_ss</v>
@@ -3621,7 +3610,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
         <f>truthStateParams!A6</f>
         <v>sig_c_ss</v>
@@ -3643,7 +3632,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="str">
         <f>truthStateParams!A7</f>
         <v>sig_meas_stx</v>
@@ -3665,7 +3654,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="str">
         <f>truthStateParams!A8</f>
         <v>sig_meas_sty</v>
@@ -3687,7 +3676,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="str">
         <f>truthStateParams!A9</f>
         <v>sig_meas_stz</v>
@@ -3709,7 +3698,7 @@
         <v>1.4544410433286079E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="43" t="str">
         <f>truthStateParams!A10</f>
         <v>sig_cu</v>
@@ -3731,7 +3720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="str">
         <f>truthStateParams!A11</f>
         <v>sig_cv</v>
@@ -3753,7 +3742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="str">
         <f>truthStateParams!A12</f>
         <v>sig_idpos</v>
@@ -3775,7 +3764,7 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="str">
         <f>truthStateParams!A13</f>
         <v>sig_loss</v>
@@ -3797,7 +3786,7 @@
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="str">
         <f>truthStateParams!A14</f>
         <v>sig_mdpos</v>
@@ -3833,17 +3822,17 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.86328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.59765625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1328125" style="6"/>
+    <col min="4" max="4" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>3</v>
       </c>
@@ -3860,7 +3849,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
         <f>truthStateInitialUncertainty!A2</f>
         <v>sig_rsx</v>
@@ -3883,7 +3872,7 @@
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
         <f>truthStateInitialUncertainty!A3</f>
         <v>sig_rsy</v>
@@ -3906,7 +3895,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="str">
         <f>truthStateInitialUncertainty!A4</f>
         <v>sig_rsz</v>
@@ -3929,7 +3918,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="str">
         <f>truthStateInitialUncertainty!A5</f>
         <v>sig_vsx</v>
@@ -3952,7 +3941,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
         <f>truthStateInitialUncertainty!A6</f>
         <v>sig_vsy</v>
@@ -3974,7 +3963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
         <f>truthStateInitialUncertainty!A7</f>
         <v>sig_vsz</v>
@@ -3996,7 +3985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
         <f>truthStateInitialUncertainty!A8</f>
         <v>sig_ax</v>
@@ -4018,7 +4007,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
         <f>truthStateInitialUncertainty!A9</f>
         <v>sig_ay</v>
@@ -4040,7 +4029,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
         <f>truthStateInitialUncertainty!A10</f>
         <v>sig_az</v>
@@ -4062,7 +4051,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="str">
         <f>truthStateInitialUncertainty!A11</f>
         <v>sig_thstx</v>
@@ -4084,7 +4073,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="str">
         <f>truthStateInitialUncertainty!A12</f>
         <v>sig_thsty</v>
@@ -4106,7 +4095,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="str">
         <f>truthStateInitialUncertainty!A13</f>
         <v>sig_thstz</v>
@@ -4128,7 +4117,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="str">
         <f>truthStateInitialUncertainty!A14</f>
         <v>sig_thcx</v>
@@ -4150,7 +4139,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="str">
         <f>truthStateInitialUncertainty!A15</f>
         <v>sig_thcy</v>
@@ -4172,7 +4161,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="str">
         <f>truthStateInitialUncertainty!A16</f>
         <v>sig_thcz</v>
@@ -4194,7 +4183,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="str">
         <f>truthStateInitialUncertainty!A17</f>
         <v>sig_gyrox</v>
@@ -4216,7 +4205,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="str">
         <f>truthStateInitialUncertainty!A18</f>
         <v>sig_gyroy</v>
@@ -4238,7 +4227,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="str">
         <f>truthStateInitialUncertainty!A19</f>
         <v>sig_gyroz</v>

</xml_diff>

<commit_message>
Fixed coordinate transformation, added a lot of debugging tools, an fixed ENU directions
</commit_message>
<xml_diff>
--- a/MATLAB Code/config.xlsx
+++ b/MATLAB Code/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\student-repos\ifroisland\MATLAB Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ikeni\Desktop\Optimal Estimation\USU_Optimal_Estimation_Project\MATLAB Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055A28B3-8F27-48DC-916E-BE0D207A5244}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB905C09-8EDB-4434-9150-0E81946036C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20715" windowHeight="13275" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -32,11 +32,22 @@
     <definedName name="min2sec">Constants!$B$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="183">
   <si>
     <t>Value</t>
   </si>
@@ -579,6 +590,12 @@
   </si>
   <si>
     <t>gravity</t>
+  </si>
+  <si>
+    <t>errorPropTestEnableCont</t>
+  </si>
+  <si>
+    <t>flag to enable continuous error propagation test</t>
   </si>
 </sst>
 </file>
@@ -614,7 +631,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -624,6 +641,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -827,7 +850,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -889,7 +912,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
@@ -901,6 +923,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1239,23 +1264,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="46" t="s">
         <v>3</v>
       </c>
@@ -1272,7 +1297,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="49" t="s">
         <v>6</v>
       </c>
@@ -1290,7 +1315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="49" t="s">
         <v>22</v>
       </c>
@@ -1308,7 +1333,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="49" t="s">
         <v>44</v>
       </c>
@@ -1326,7 +1351,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="49" t="s">
         <v>12</v>
       </c>
@@ -1344,7 +1369,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="49" t="s">
         <v>47</v>
       </c>
@@ -1362,7 +1387,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="49" t="s">
         <v>92</v>
       </c>
@@ -1381,11 +1406,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
+    <row r="8" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="52">
+      <c r="B8" s="73">
         <v>0</v>
       </c>
       <c r="C8" s="49" t="s">
@@ -1395,85 +1420,85 @@
         <v>39</v>
       </c>
       <c r="E8" s="51">
-        <f t="shared" ref="E8:E13" si="1">B8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="52">
+        <f t="shared" ref="E8:E14" si="1">B8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B9" s="73">
         <v>0</v>
       </c>
       <c r="C9" s="49" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="49" t="s">
-        <v>21</v>
+        <v>182</v>
       </c>
       <c r="E9" s="51">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="61" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="52">
-        <v>0</v>
+    <row r="10" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="72" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="73">
+        <v>1</v>
       </c>
       <c r="C10" s="49" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="49" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E10" s="51">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="62" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="74" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="73">
+        <v>0</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="51">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" s="61" t="s">
         <v>139</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B12" s="2">
         <v>2</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C12" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="D11" s="49" t="s">
+      <c r="D12" s="49" t="s">
         <v>141</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E12" s="1">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" s="49" t="s">
         <v>142</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1</v>
-      </c>
-      <c r="C12" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="49" t="s">
-        <v>144</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="49" t="s">
-        <v>143</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
@@ -1482,177 +1507,195 @@
         <v>5</v>
       </c>
       <c r="D13" s="49" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="49" t="s">
+        <v>143</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" s="49" t="s">
         <v>146</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B15" s="2">
         <v>122</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C15" s="49" t="s">
         <v>147</v>
       </c>
-      <c r="D14" s="49" t="s">
+      <c r="D15" s="49" t="s">
         <v>148</v>
       </c>
-      <c r="E14" s="1">
-        <f>B14*1000000</f>
+      <c r="E15" s="1">
+        <f>B15*1000000</f>
         <v>122000000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="49" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" s="49" t="s">
         <v>149</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B16" s="2">
         <v>299702547</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C16" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="D15" s="49" t="s">
+      <c r="D16" s="49" t="s">
         <v>150</v>
       </c>
-      <c r="E15" s="1">
-        <f t="shared" ref="E15:E22" si="2">B15</f>
+      <c r="E16" s="1">
+        <f t="shared" ref="E16:E23" si="2">B16</f>
         <v>299702547</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="49" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" s="49" t="s">
         <v>156</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B17" s="2">
         <v>0.5</v>
       </c>
-      <c r="C16" s="64" t="s">
+      <c r="C17" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="64" t="s">
+      <c r="D17" s="63" t="s">
         <v>157</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E17" s="1">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="49" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" s="49" t="s">
         <v>155</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B18" s="2">
         <v>1</v>
       </c>
-      <c r="C17" s="49" t="s">
+      <c r="C18" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="64" t="s">
+      <c r="D18" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E18" s="1">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="49" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" s="49" t="s">
         <v>154</v>
       </c>
-      <c r="B18" s="63">
-        <v>0</v>
-      </c>
-      <c r="C18" s="49" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="64" t="s">
-        <v>159</v>
-      </c>
-      <c r="E18" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="49" t="s">
-        <v>153</v>
-      </c>
-      <c r="B19" s="2">
-        <v>-0.5</v>
+      <c r="B19" s="62">
+        <v>0</v>
       </c>
       <c r="C19" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="64" t="s">
-        <v>160</v>
+      <c r="D19" s="63" t="s">
+        <v>159</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" s="49" t="s">
+        <v>153</v>
+      </c>
+      <c r="B20" s="2">
         <v>-0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="49" t="s">
-        <v>152</v>
-      </c>
-      <c r="B20" s="2">
-        <v>1</v>
       </c>
       <c r="C20" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="64" t="s">
-        <v>161</v>
+      <c r="D20" s="63" t="s">
+        <v>160</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="2"/>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" s="49" t="s">
+        <v>152</v>
+      </c>
+      <c r="B21" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="49" t="s">
-        <v>151</v>
-      </c>
-      <c r="B21" s="2">
-        <v>0</v>
-      </c>
-      <c r="C21" s="64" t="s">
+      <c r="C21" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="64" t="s">
-        <v>162</v>
+      <c r="D21" s="63" t="s">
+        <v>161</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="64" t="s">
-        <v>132</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" s="49" t="s">
+        <v>151</v>
       </c>
       <c r="B22" s="2">
-        <v>9.81</v>
-      </c>
-      <c r="C22" s="71" t="s">
-        <v>179</v>
-      </c>
-      <c r="D22" s="72" t="s">
-        <v>180</v>
+        <v>0</v>
+      </c>
+      <c r="C22" s="63" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="63" t="s">
+        <v>162</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" s="63" t="s">
+        <v>132</v>
+      </c>
+      <c r="B23" s="2">
         <v>9.81</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C26" s="45"/>
+      <c r="C23" s="70" t="s">
+        <v>179</v>
+      </c>
+      <c r="D23" s="71" t="s">
+        <v>180</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="2"/>
+        <v>9.81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C27" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1668,12 +1711,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1681,7 +1724,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1689,7 +1732,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1698,7 +1741,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1706,7 +1749,7 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>107</v>
       </c>
@@ -1724,18 +1767,18 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
@@ -1752,7 +1795,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>174</v>
       </c>
@@ -1770,7 +1813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
         <v>173</v>
       </c>
@@ -1788,14 +1831,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" s="64" t="s">
         <v>170</v>
       </c>
-      <c r="B4" s="66">
+      <c r="B4" s="65">
         <v>5</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="66" t="s">
         <v>108</v>
       </c>
       <c r="D4" s="32"/>
@@ -1804,14 +1847,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="65" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" s="64" t="s">
         <v>178</v>
       </c>
-      <c r="B5" s="66">
-        <v>0</v>
-      </c>
-      <c r="C5" s="67" t="s">
+      <c r="B5" s="65">
+        <v>0</v>
+      </c>
+      <c r="C5" s="66" t="s">
         <v>163</v>
       </c>
       <c r="D5" s="29"/>
@@ -1820,23 +1863,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="65" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="66">
-        <v>5</v>
-      </c>
-      <c r="C6" s="67" t="s">
+      <c r="B6" s="65">
+        <v>0</v>
+      </c>
+      <c r="C6" s="66" t="s">
         <v>163</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="30">
         <f>RADIANS(B6)</f>
-        <v>8.7266462599716474E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="58" t="s">
         <v>133</v>
       </c>
@@ -1854,11 +1897,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="59" t="s">
         <v>135</v>
       </c>
-      <c r="B8" s="68">
+      <c r="B8" s="67">
         <v>0</v>
       </c>
       <c r="C8" t="s">
@@ -1872,11 +1915,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="60" t="s">
         <v>136</v>
       </c>
-      <c r="B9" s="69">
+      <c r="B9" s="68">
         <v>0</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -1890,11 +1933,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="59" t="s">
         <v>134</v>
       </c>
-      <c r="B10" s="70">
+      <c r="B10" s="69">
         <v>0</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1908,11 +1951,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="59" t="s">
         <v>137</v>
       </c>
-      <c r="B11" s="68">
+      <c r="B11" s="67">
         <v>0</v>
       </c>
       <c r="C11" t="s">
@@ -1926,11 +1969,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="60" t="s">
         <v>138</v>
       </c>
-      <c r="B12" s="69">
+      <c r="B12" s="68">
         <v>0</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -1944,11 +1987,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="B13" s="70">
+      <c r="B13" s="69">
         <v>0</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -1962,11 +2005,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="B14" s="68">
+      <c r="B14" s="67">
         <v>0</v>
       </c>
       <c r="C14" t="s">
@@ -1980,11 +2023,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="B15" s="69">
+      <c r="B15" s="68">
         <v>0</v>
       </c>
       <c r="C15" s="8" t="s">
@@ -1998,55 +2041,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="E16" s="57"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B17" s="16"/>
       <c r="C17" s="6"/>
       <c r="E17" s="39"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B18" s="8"/>
       <c r="C18" s="17"/>
       <c r="E18" s="40"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="E19" s="39"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B20" s="16"/>
       <c r="C20" s="6"/>
       <c r="E20" s="39"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="E21" s="40"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B22" s="53"/>
       <c r="C22" s="16"/>
       <c r="E22" s="55"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B23" s="53"/>
       <c r="C23" s="16"/>
       <c r="E23" s="55"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B24" s="42"/>
       <c r="C24" s="17"/>
       <c r="E24" s="56"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
       <c r="D28" s="6"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D35" s="6"/>
     </row>
   </sheetData>
@@ -2060,18 +2103,18 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.59765625" customWidth="1"/>
+    <col min="5" max="5" width="13.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="35" t="s">
         <v>3</v>
       </c>
@@ -2088,12 +2131,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B2" s="4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="4" t="str">
         <f>truthStateInitialUncertainty!C2</f>
@@ -2104,11 +2147,11 @@
       </c>
       <c r="E2" s="57">
         <f t="shared" ref="E2:E7" si="0">B2</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>86</v>
       </c>
@@ -2128,7 +2171,7 @@
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>87</v>
       </c>
@@ -2148,7 +2191,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>88</v>
       </c>
@@ -2168,7 +2211,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
         <v>89</v>
       </c>
@@ -2188,7 +2231,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>90</v>
       </c>
@@ -2208,7 +2251,7 @@
       </c>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
         <v>129</v>
       </c>
@@ -2227,7 +2270,7 @@
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
         <v>130</v>
       </c>
@@ -2246,7 +2289,7 @@
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
         <v>131</v>
       </c>
@@ -2265,7 +2308,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
         <v>121</v>
       </c>
@@ -2284,7 +2327,7 @@
       </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
         <v>122</v>
       </c>
@@ -2303,7 +2346,7 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
         <v>123</v>
       </c>
@@ -2322,7 +2365,7 @@
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
         <v>26</v>
       </c>
@@ -2342,7 +2385,7 @@
       </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
         <v>28</v>
       </c>
@@ -2361,7 +2404,7 @@
         <v>9.6962736221907197E-6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>29</v>
       </c>
@@ -2380,7 +2423,7 @@
         <v>1.454441043328608E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="18" t="s">
         <v>125</v>
       </c>
@@ -2398,7 +2441,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="18" t="s">
         <v>126</v>
       </c>
@@ -2416,7 +2459,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="19" t="s">
         <v>127</v>
       </c>
@@ -2445,17 +2488,17 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -2472,7 +2515,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>176</v>
       </c>
@@ -2489,7 +2532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>177</v>
       </c>
@@ -2506,7 +2549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>175</v>
       </c>
@@ -2523,7 +2566,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>178</v>
       </c>
@@ -2540,7 +2583,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>115</v>
       </c>
@@ -2557,7 +2600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>116</v>
       </c>
@@ -2574,7 +2617,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
         <v>49</v>
       </c>
@@ -2591,7 +2634,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
         <v>117</v>
       </c>
@@ -2608,7 +2651,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
@@ -2628,7 +2671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="7" t="s">
         <v>43</v>
       </c>
@@ -2662,14 +2705,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -2686,7 +2729,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -2703,7 +2746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>31</v>
       </c>
@@ -2720,7 +2763,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
@@ -2737,7 +2780,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>116</v>
       </c>
@@ -2754,7 +2797,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
         <v>49</v>
       </c>
@@ -2771,7 +2814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
         <v>117</v>
       </c>
@@ -2788,7 +2831,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
         <v>42</v>
       </c>
@@ -2809,7 +2852,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="7" t="s">
         <v>43</v>
       </c>
@@ -2841,17 +2884,17 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="35" t="s">
         <v>3</v>
       </c>
@@ -2868,7 +2911,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>93</v>
       </c>
@@ -2887,7 +2930,7 @@
         <v>1.6000000000000003E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
@@ -2906,7 +2949,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -2924,7 +2967,7 @@
         <v>4.8481368110953598E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>71</v>
       </c>
@@ -2942,7 +2985,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
         <v>72</v>
       </c>
@@ -2960,7 +3003,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="18" t="s">
         <v>73</v>
       </c>
@@ -2978,7 +3021,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="18" t="s">
         <v>74</v>
       </c>
@@ -2996,7 +3039,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="18" t="s">
         <v>75</v>
       </c>
@@ -3014,7 +3057,7 @@
         <v>1.4544410433286079E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="43" t="s">
         <v>97</v>
       </c>
@@ -3032,7 +3075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="19" t="s">
         <v>98</v>
       </c>
@@ -3050,7 +3093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="18" t="s">
         <v>101</v>
       </c>
@@ -3068,7 +3111,7 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="18" t="s">
         <v>103</v>
       </c>
@@ -3086,7 +3129,7 @@
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="18" t="s">
         <v>105</v>
       </c>
@@ -3118,17 +3161,17 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.265625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="4" width="51.265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.73046875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.3984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1328125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
@@ -3145,7 +3188,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>55</v>
       </c>
@@ -3163,7 +3206,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>57</v>
       </c>
@@ -3181,7 +3224,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>58</v>
       </c>
@@ -3199,7 +3242,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>59</v>
       </c>
@@ -3217,7 +3260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
         <v>62</v>
       </c>
@@ -3235,7 +3278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>63</v>
       </c>
@@ -3253,7 +3296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
         <v>76</v>
       </c>
@@ -3271,7 +3314,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
         <v>77</v>
       </c>
@@ -3289,7 +3332,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
         <v>78</v>
       </c>
@@ -3307,7 +3350,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
         <v>82</v>
       </c>
@@ -3326,7 +3369,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="18" t="s">
         <v>83</v>
       </c>
@@ -3345,7 +3388,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="18" t="s">
         <v>84</v>
       </c>
@@ -3364,7 +3407,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="18" t="s">
         <v>79</v>
       </c>
@@ -3383,7 +3426,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="18" t="s">
         <v>80</v>
       </c>
@@ -3402,7 +3445,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="16" t="s">
         <v>81</v>
       </c>
@@ -3421,7 +3464,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
         <v>67</v>
       </c>
@@ -3440,7 +3483,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="5" t="s">
         <v>69</v>
       </c>
@@ -3459,7 +3502,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="7" t="s">
         <v>70</v>
       </c>
@@ -3490,18 +3533,18 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.73046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.86328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.73046875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="14.3984375" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="7" max="16384" width="9.1328125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="35" t="s">
         <v>3</v>
       </c>
@@ -3518,7 +3561,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="str">
         <f>truthStateParams!A2</f>
         <v>Q_grav</v>
@@ -3541,7 +3584,7 @@
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="str">
         <f>truthStateParams!A3</f>
         <v>sig_gyro_ss</v>
@@ -3564,7 +3607,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="str">
         <f>truthStateParams!A4</f>
         <v>arw</v>
@@ -3587,7 +3630,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="str">
         <f>truthStateParams!A5</f>
         <v>sig_st_ss</v>
@@ -3610,7 +3653,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="str">
         <f>truthStateParams!A6</f>
         <v>sig_c_ss</v>
@@ -3632,7 +3675,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="18" t="str">
         <f>truthStateParams!A7</f>
         <v>sig_meas_stx</v>
@@ -3654,7 +3697,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="18" t="str">
         <f>truthStateParams!A8</f>
         <v>sig_meas_sty</v>
@@ -3676,7 +3719,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="18" t="str">
         <f>truthStateParams!A9</f>
         <v>sig_meas_stz</v>
@@ -3698,7 +3741,7 @@
         <v>1.4544410433286079E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="43" t="str">
         <f>truthStateParams!A10</f>
         <v>sig_cu</v>
@@ -3720,7 +3763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="19" t="str">
         <f>truthStateParams!A11</f>
         <v>sig_cv</v>
@@ -3742,7 +3785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="19" t="str">
         <f>truthStateParams!A12</f>
         <v>sig_idpos</v>
@@ -3764,7 +3807,7 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="19" t="str">
         <f>truthStateParams!A13</f>
         <v>sig_loss</v>
@@ -3786,7 +3829,7 @@
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="19" t="str">
         <f>truthStateParams!A14</f>
         <v>sig_mdpos</v>
@@ -3822,17 +3865,17 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.265625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="4" width="51.265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.86328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.59765625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1328125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="35" t="s">
         <v>3</v>
       </c>
@@ -3849,7 +3892,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="str">
         <f>truthStateInitialUncertainty!A2</f>
         <v>sig_rsx</v>
@@ -3872,7 +3915,7 @@
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="str">
         <f>truthStateInitialUncertainty!A3</f>
         <v>sig_rsy</v>
@@ -3895,7 +3938,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="str">
         <f>truthStateInitialUncertainty!A4</f>
         <v>sig_rsz</v>
@@ -3918,7 +3961,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="str">
         <f>truthStateInitialUncertainty!A5</f>
         <v>sig_vsx</v>
@@ -3941,7 +3984,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="str">
         <f>truthStateInitialUncertainty!A6</f>
         <v>sig_vsy</v>
@@ -3963,7 +4006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="str">
         <f>truthStateInitialUncertainty!A7</f>
         <v>sig_vsz</v>
@@ -3985,7 +4028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="str">
         <f>truthStateInitialUncertainty!A8</f>
         <v>sig_ax</v>
@@ -4007,7 +4050,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="str">
         <f>truthStateInitialUncertainty!A9</f>
         <v>sig_ay</v>
@@ -4029,7 +4072,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="str">
         <f>truthStateInitialUncertainty!A10</f>
         <v>sig_az</v>
@@ -4051,7 +4094,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="str">
         <f>truthStateInitialUncertainty!A11</f>
         <v>sig_thstx</v>
@@ -4073,7 +4116,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="str">
         <f>truthStateInitialUncertainty!A12</f>
         <v>sig_thsty</v>
@@ -4095,7 +4138,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="str">
         <f>truthStateInitialUncertainty!A13</f>
         <v>sig_thstz</v>
@@ -4117,7 +4160,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="str">
         <f>truthStateInitialUncertainty!A14</f>
         <v>sig_thcx</v>
@@ -4139,7 +4182,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="str">
         <f>truthStateInitialUncertainty!A15</f>
         <v>sig_thcy</v>
@@ -4161,7 +4204,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="5" t="str">
         <f>truthStateInitialUncertainty!A16</f>
         <v>sig_thcz</v>
@@ -4183,7 +4226,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="str">
         <f>truthStateInitialUncertainty!A17</f>
         <v>sig_gyrox</v>
@@ -4205,7 +4248,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="5" t="str">
         <f>truthStateInitialUncertainty!A18</f>
         <v>sig_gyroy</v>
@@ -4227,7 +4270,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="7" t="str">
         <f>truthStateInitialUncertainty!A19</f>
         <v>sig_gyroz</v>

</xml_diff>

<commit_message>
Made plots prettier, updated system inputs to cause sinusoid-like trajectory
</commit_message>
<xml_diff>
--- a/MATLAB Code/config.xlsx
+++ b/MATLAB Code/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ikeni\Desktop\Optimal Estimation\USU_Optimal_Estimation_Project\MATLAB Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB905C09-8EDB-4434-9150-0E81946036C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AF3AC7-01FA-463D-A2F7-B5DC92AD9F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="885" yWindow="2633" windowWidth="15390" windowHeight="9532" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -602,11 +602,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.00000000E+00"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0000000"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -850,7 +851,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -918,14 +919,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1266,8 +1268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1407,10 +1409,10 @@
       </c>
     </row>
     <row r="8" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="72" t="s">
+      <c r="A8" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="73">
+      <c r="B8" s="70">
         <v>0</v>
       </c>
       <c r="C8" s="49" t="s">
@@ -1425,10 +1427,10 @@
       </c>
     </row>
     <row r="9" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="72" t="s">
+      <c r="A9" s="69" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="73">
+      <c r="B9" s="70">
         <v>0</v>
       </c>
       <c r="C9" s="49" t="s">
@@ -1443,11 +1445,11 @@
       </c>
     </row>
     <row r="10" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="72" t="s">
+      <c r="A10" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="73">
-        <v>1</v>
+      <c r="B10" s="70">
+        <v>0</v>
       </c>
       <c r="C10" s="49" t="s">
         <v>4</v>
@@ -1457,14 +1459,14 @@
       </c>
       <c r="E10" s="51">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="74" t="s">
+      <c r="A11" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="73">
+      <c r="B11" s="70">
         <v>0</v>
       </c>
       <c r="C11" s="49" t="s">
@@ -1683,10 +1685,10 @@
       <c r="B23" s="2">
         <v>9.81</v>
       </c>
-      <c r="C23" s="70" t="s">
+      <c r="C23" s="67" t="s">
         <v>179</v>
       </c>
-      <c r="D23" s="71" t="s">
+      <c r="D23" s="68" t="s">
         <v>180</v>
       </c>
       <c r="E23" s="1">
@@ -1767,13 +1769,13 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.19921875" customWidth="1"/>
     <col min="4" max="4" width="72.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.3984375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1901,7 +1903,7 @@
       <c r="A8" s="59" t="s">
         <v>135</v>
       </c>
-      <c r="B8" s="67">
+      <c r="B8" s="73">
         <v>0</v>
       </c>
       <c r="C8" t="s">
@@ -1919,7 +1921,7 @@
       <c r="A9" s="60" t="s">
         <v>136</v>
       </c>
-      <c r="B9" s="68">
+      <c r="B9" s="72">
         <v>0</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -1937,7 +1939,7 @@
       <c r="A10" s="59" t="s">
         <v>134</v>
       </c>
-      <c r="B10" s="69">
+      <c r="B10" s="74">
         <v>0</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1947,7 +1949,7 @@
         <v>167</v>
       </c>
       <c r="E10" s="57">
-        <f t="shared" ref="E10:E11" si="3">RADIANS(B10)</f>
+        <f>RADIANS(B10)/hr2sec</f>
         <v>0</v>
       </c>
     </row>
@@ -1955,7 +1957,7 @@
       <c r="A11" s="59" t="s">
         <v>137</v>
       </c>
-      <c r="B11" s="67">
+      <c r="B11" s="73">
         <v>0</v>
       </c>
       <c r="C11" t="s">
@@ -1965,7 +1967,7 @@
         <v>168</v>
       </c>
       <c r="E11" s="57">
-        <f t="shared" si="3"/>
+        <f>RADIANS(B11)/hr2sec</f>
         <v>0</v>
       </c>
     </row>
@@ -1973,7 +1975,7 @@
       <c r="A12" s="60" t="s">
         <v>138</v>
       </c>
-      <c r="B12" s="68">
+      <c r="B12" s="72">
         <v>0</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -1983,7 +1985,7 @@
         <v>169</v>
       </c>
       <c r="E12" s="57">
-        <f>RADIANS(B12)</f>
+        <f>RADIANS(B12)/hr2sec</f>
         <v>0</v>
       </c>
     </row>
@@ -1991,7 +1993,7 @@
       <c r="A13" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="B13" s="69">
+      <c r="B13" s="74">
         <v>0</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -2000,8 +2002,8 @@
       <c r="D13" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="E13" s="39">
-        <f>RADIANS(B13)</f>
+      <c r="E13" s="75">
+        <f>B13</f>
         <v>0</v>
       </c>
     </row>
@@ -2009,8 +2011,8 @@
       <c r="A14" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="B14" s="67">
-        <v>0</v>
+      <c r="B14" s="73">
+        <v>20</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -2018,17 +2020,17 @@
       <c r="D14" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="E14" s="40">
-        <f>RADIANS(B14)</f>
-        <v>0</v>
+      <c r="E14" s="75">
+        <f t="shared" ref="E14:E15" si="3">B14</f>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="B15" s="68">
-        <v>0</v>
+      <c r="B15" s="72">
+        <v>-0.15</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>8</v>
@@ -2036,9 +2038,9 @@
       <c r="D15" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="E15" s="57">
-        <f>RADIANS(B15)</f>
-        <v>0</v>
+      <c r="E15" s="75">
+        <f t="shared" si="3"/>
+        <v>-0.15</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Completed linear measurement modeling
</commit_message>
<xml_diff>
--- a/MATLAB Code/config.xlsx
+++ b/MATLAB Code/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ikeni\Desktop\Optimal Estimation\USU_Optimal_Estimation_Project\MATLAB Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AF3AC7-01FA-463D-A2F7-B5DC92AD9F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB630F15-1975-4606-9C43-62B8C9440E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="885" yWindow="2633" windowWidth="15390" windowHeight="9532" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="187">
   <si>
     <t>Value</t>
   </si>
@@ -596,6 +596,18 @@
   </si>
   <si>
     <t>flag to enable continuous error propagation test</t>
+  </si>
+  <si>
+    <t>process_GPS_enable</t>
+  </si>
+  <si>
+    <t>process_IBC_enable</t>
+  </si>
+  <si>
+    <t>flag to enable processing of IBC measurement for Kalman update</t>
+  </si>
+  <si>
+    <t>flag to enable processing of GPS measurement for Kalman update</t>
   </si>
 </sst>
 </file>
@@ -607,7 +619,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0000000"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -851,7 +863,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -924,10 +936,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1266,10 +1282,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1422,7 +1438,7 @@
         <v>39</v>
       </c>
       <c r="E8" s="51">
-        <f t="shared" ref="E8:E14" si="1">B8</f>
+        <f t="shared" ref="E8:E16" si="1">B8</f>
         <v>0</v>
       </c>
     </row>
@@ -1467,7 +1483,7 @@
         <v>40</v>
       </c>
       <c r="B11" s="70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="49" t="s">
         <v>4</v>
@@ -1477,227 +1493,263 @@
       </c>
       <c r="E11" s="51">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="61" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="79" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="76" t="s">
+        <v>184</v>
+      </c>
+      <c r="B12" s="77">
+        <v>1</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="49" t="s">
+        <v>185</v>
+      </c>
+      <c r="E12" s="78">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="79" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="76" t="s">
+        <v>183</v>
+      </c>
+      <c r="B13" s="77">
+        <v>1</v>
+      </c>
+      <c r="C13" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="E13" s="78">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" s="61" t="s">
         <v>139</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B14" s="2">
         <v>2</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C14" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="D12" s="49" t="s">
+      <c r="D14" s="49" t="s">
         <v>141</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E14" s="1">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="49" t="s">
-        <v>142</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="49" t="s">
-        <v>144</v>
-      </c>
-      <c r="E13" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="49" t="s">
-        <v>143</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
-      <c r="C14" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="49" t="s">
-        <v>145</v>
-      </c>
-      <c r="E14" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="49" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B15" s="2">
-        <v>122</v>
+        <v>1</v>
       </c>
       <c r="C15" s="49" t="s">
-        <v>147</v>
+        <v>5</v>
       </c>
       <c r="D15" s="49" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E15" s="1">
-        <f>B15*1000000</f>
-        <v>122000000</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="49" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B16" s="2">
-        <v>299702547</v>
+        <v>1</v>
       </c>
       <c r="C16" s="49" t="s">
-        <v>108</v>
+        <v>5</v>
       </c>
       <c r="D16" s="49" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" ref="E16:E23" si="2">B16</f>
-        <v>299702547</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="49" t="s">
+        <v>146</v>
+      </c>
+      <c r="B17" s="2">
+        <v>122</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="E17" s="1">
+        <f>B17*1000000</f>
+        <v>122000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="B18" s="2">
+        <v>299702547</v>
+      </c>
+      <c r="C18" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="49" t="s">
+        <v>150</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" ref="E18:E25" si="2">B18</f>
+        <v>299702547</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" s="49" t="s">
         <v>156</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B19" s="2">
         <v>0.5</v>
       </c>
-      <c r="C17" s="63" t="s">
+      <c r="C19" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="63" t="s">
+      <c r="D19" s="63" t="s">
         <v>157</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E19" s="1">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A18" s="49" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" s="49" t="s">
         <v>155</v>
       </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
-      <c r="C18" s="49" t="s">
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="63" t="s">
+      <c r="D20" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E20" s="1">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A19" s="49" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" s="49" t="s">
         <v>154</v>
       </c>
-      <c r="B19" s="62">
+      <c r="B21" s="62">
         <v>0</v>
       </c>
-      <c r="C19" s="49" t="s">
+      <c r="C21" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="63" t="s">
+      <c r="D21" s="63" t="s">
         <v>159</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E21" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A20" s="49" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" s="49" t="s">
         <v>153</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B22" s="2">
         <v>-0.5</v>
       </c>
-      <c r="C20" s="49" t="s">
+      <c r="C22" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="63" t="s">
+      <c r="D22" s="63" t="s">
         <v>160</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E22" s="1">
         <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A21" s="49" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="B21" s="2">
-        <v>1</v>
-      </c>
-      <c r="C21" s="49" t="s">
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="63" t="s">
+      <c r="D23" s="63" t="s">
         <v>161</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E23" s="1">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A22" s="49" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" s="49" t="s">
         <v>151</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B24" s="2">
         <v>0</v>
       </c>
-      <c r="C22" s="63" t="s">
+      <c r="C24" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="63" t="s">
+      <c r="D24" s="63" t="s">
         <v>162</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E24" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A23" s="63" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" s="63" t="s">
         <v>132</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B25" s="2">
         <v>9.81</v>
       </c>
-      <c r="C23" s="67" t="s">
+      <c r="C25" s="67" t="s">
         <v>179</v>
       </c>
-      <c r="D23" s="68" t="s">
+      <c r="D25" s="68" t="s">
         <v>180</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E25" s="1">
         <f t="shared" si="2"/>
         <v>9.81</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C27" s="45"/>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C29" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1769,7 +1821,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2105,7 +2157,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2138,7 +2190,7 @@
         <v>85</v>
       </c>
       <c r="B2" s="4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C2" s="4" t="str">
         <f>truthStateInitialUncertainty!C2</f>
@@ -2149,7 +2201,7 @@
       </c>
       <c r="E2" s="57">
         <f t="shared" ref="E2:E7" si="0">B2</f>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F2" s="6"/>
     </row>

</xml_diff>

<commit_message>
Fixed GPS linearization with GPS offset, finished documentation for linear measurement modeling
</commit_message>
<xml_diff>
--- a/MATLAB Code/config.xlsx
+++ b/MATLAB Code/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ikeni\Desktop\Optimal Estimation\USU_Optimal_Estimation_Project\MATLAB Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB630F15-1975-4606-9C43-62B8C9440E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C99437E-6305-46A9-8CCD-1429B608A649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="193">
   <si>
     <t>Value</t>
   </si>
@@ -608,6 +608,24 @@
   </si>
   <si>
     <t>flag to enable processing of GPS measurement for Kalman update</t>
+  </si>
+  <si>
+    <t>r_gps_x</t>
+  </si>
+  <si>
+    <t>r_gps_y</t>
+  </si>
+  <si>
+    <t>r_gps_z</t>
+  </si>
+  <si>
+    <t>x component of gps position wrt to body frame</t>
+  </si>
+  <si>
+    <t>y component of gps position wrt to body frame</t>
+  </si>
+  <si>
+    <t>z component of gps position wrt to body frame</t>
   </si>
 </sst>
 </file>
@@ -1285,7 +1303,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1618,7 +1636,7 @@
         <v>150</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" ref="E18:E25" si="2">B18</f>
+        <f t="shared" ref="E18:E28" si="2">B18</f>
         <v>299702547</v>
       </c>
     </row>
@@ -1746,6 +1764,51 @@
       <c r="E25" s="1">
         <f t="shared" si="2"/>
         <v>9.81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26" s="67" t="s">
+        <v>187</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0</v>
+      </c>
+      <c r="D26" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" s="67" t="s">
+        <v>188</v>
+      </c>
+      <c r="B27" s="2">
+        <v>-0.25</v>
+      </c>
+      <c r="D27" s="63" t="s">
+        <v>191</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28" s="67" t="s">
+        <v>189</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
+      <c r="D28" s="63" t="s">
+        <v>192</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
First attempt at full Kalman filter, has issues with state and covariance updates
</commit_message>
<xml_diff>
--- a/MATLAB Code/config.xlsx
+++ b/MATLAB Code/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ikeni\Desktop\Optimal Estimation\USU_Optimal_Estimation_Project\MATLAB Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117A3E10-9D39-4E98-8600-0BA2AB02FB0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5A09AF-B543-41D0-93E3-4CEBC1111CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="894" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2415" yWindow="3540" windowWidth="15390" windowHeight="9540" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -166,9 +166,6 @@
     <t>flag to enable checking of error definition consistency</t>
   </si>
   <si>
-    <t>measLinerizationCheckEnable</t>
-  </si>
-  <si>
     <t>flag to enable checking of measurement linearization</t>
   </si>
   <si>
@@ -448,12 +445,6 @@
     <t>gravity</t>
   </si>
   <si>
-    <t>errorPropTestEnableCont</t>
-  </si>
-  <si>
-    <t>flag to enable continuous error propagation test</t>
-  </si>
-  <si>
     <t>process_GPS_enable</t>
   </si>
   <si>
@@ -532,9 +523,6 @@
     <t>sig_gps_z</t>
   </si>
   <si>
-    <t>sig_ibc</t>
-  </si>
-  <si>
     <t>V</t>
   </si>
   <si>
@@ -646,13 +634,25 @@
     <t>3-sigma initial attitude uncertainty</t>
   </si>
   <si>
-    <t>3-sigma ibc measurement noise</t>
-  </si>
-  <si>
-    <t>noiseOn</t>
-  </si>
-  <si>
-    <t>flag to enable synthesis of noise</t>
+    <t>sig_pdoa</t>
+  </si>
+  <si>
+    <t>3-sigma pdoa measurement noise</t>
+  </si>
+  <si>
+    <t>processNoiseOn</t>
+  </si>
+  <si>
+    <t>measurementNoiseOn</t>
+  </si>
+  <si>
+    <t>flag to enable synthesis of measurement noise</t>
+  </si>
+  <si>
+    <t>flag to enable synthesis of process noise</t>
+  </si>
+  <si>
+    <t>measLinearizationCheckEnable</t>
   </si>
 </sst>
 </file>
@@ -710,7 +710,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -958,21 +958,6 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -1085,7 +1070,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1165,31 +1150,29 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1537,8 +1520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:B22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1552,33 +1535,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="85" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="84" t="s">
+      <c r="B1" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="84" t="s">
+      <c r="D1" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="86" t="s">
-        <v>57</v>
+      <c r="E1" s="84" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="87" t="s">
-        <v>166</v>
-      </c>
-      <c r="B2" s="88">
+      <c r="A2" s="85" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="86">
         <v>0.01</v>
       </c>
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="87" t="s">
+      <c r="D2" s="85" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="44">
@@ -1588,10 +1571,10 @@
     </row>
     <row r="3" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="42" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B3" s="43">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C3" s="42" t="s">
         <v>5</v>
@@ -1601,7 +1584,7 @@
       </c>
       <c r="E3" s="44">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.45">
@@ -1615,7 +1598,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="44">
         <f t="shared" si="0"/>
@@ -1624,7 +1607,7 @@
     </row>
     <row r="5" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="43">
         <v>10</v>
@@ -1633,7 +1616,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" s="44">
         <f t="shared" si="0"/>
@@ -1660,7 +1643,7 @@
     </row>
     <row r="7" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="45">
         <v>12</v>
@@ -1669,7 +1652,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="44">
         <f>B7</f>
@@ -1678,10 +1661,10 @@
     </row>
     <row r="8" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="76" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="77">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="C8" s="42" t="s">
         <v>4</v>
@@ -1691,7 +1674,7 @@
       </c>
       <c r="E8" s="44">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.45">
@@ -1714,7 +1697,7 @@
     </row>
     <row r="10" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="79" t="s">
-        <v>133</v>
+        <v>19</v>
       </c>
       <c r="B10" s="80">
         <v>0</v>
@@ -1723,7 +1706,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="42" t="s">
-        <v>134</v>
+        <v>20</v>
       </c>
       <c r="E10" s="44">
         <f t="shared" si="1"/>
@@ -1731,53 +1714,53 @@
       </c>
     </row>
     <row r="11" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="81" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="82">
+      <c r="A11" s="74" t="s">
+        <v>201</v>
+      </c>
+      <c r="B11" s="75">
         <v>0</v>
       </c>
       <c r="C11" s="66" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="42" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="E11" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="74" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="75">
-        <v>0</v>
+    <row r="12" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="70" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" s="71">
+        <v>1</v>
       </c>
       <c r="C12" s="66" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="44">
+        <v>134</v>
+      </c>
+      <c r="E12" s="64">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="70" t="s">
-        <v>136</v>
-      </c>
-      <c r="B13" s="71">
+      <c r="A13" s="72" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" s="73">
         <v>0</v>
       </c>
       <c r="C13" s="66" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E13" s="64">
         <f t="shared" si="1"/>
@@ -1785,107 +1768,107 @@
       </c>
     </row>
     <row r="14" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="72" t="s">
-        <v>135</v>
-      </c>
-      <c r="B14" s="73">
+      <c r="A14" s="68" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" s="69">
         <v>0</v>
       </c>
       <c r="C14" s="66" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="42" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="E14" s="64">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="68" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" s="70" t="s">
         <v>145</v>
       </c>
-      <c r="B15" s="69">
+      <c r="B15" s="71">
         <v>0</v>
       </c>
       <c r="C15" s="66" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="42" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E15" s="64">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="E15:E16" si="2">B15</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="70" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B16" s="71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="66" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="42" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E16" s="64">
-        <f t="shared" ref="E16:E17" si="2">B16</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A17" s="70" t="s">
+      <c r="A17" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="B17" s="71">
-        <v>1</v>
+      <c r="B17" s="73">
+        <v>0</v>
       </c>
       <c r="C17" s="66" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="42" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E17" s="64">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" ref="E17:E19" si="3">B17</f>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="72" t="s">
-        <v>149</v>
+        <v>198</v>
       </c>
       <c r="B18" s="73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="66" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="42" t="s">
-        <v>150</v>
+        <v>199</v>
       </c>
       <c r="E18" s="64">
-        <f t="shared" ref="E18:E19" si="3">B18</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A19" s="109" t="s">
-        <v>200</v>
-      </c>
-      <c r="B19" s="110">
+      <c r="A19" s="107" t="s">
+        <v>197</v>
+      </c>
+      <c r="B19" s="108">
         <v>1</v>
       </c>
       <c r="C19" s="66" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E19" s="64">
         <f t="shared" si="3"/>
@@ -1894,16 +1877,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="67" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B20" s="2">
         <v>2</v>
       </c>
       <c r="C20" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="42" t="s">
         <v>92</v>
-      </c>
-      <c r="D20" s="42" t="s">
-        <v>93</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="1"/>
@@ -1912,52 +1895,52 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B21" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C21" s="42" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B22" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C22" s="42" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B23" s="2">
         <v>122</v>
       </c>
       <c r="C23" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="42" t="s">
         <v>99</v>
-      </c>
-      <c r="D23" s="42" t="s">
-        <v>100</v>
       </c>
       <c r="E23" s="1">
         <f>B23*1000000</f>
@@ -1966,16 +1949,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="76" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B24" s="2">
         <v>299702547</v>
       </c>
       <c r="C24" s="76" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D24" s="76" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" ref="E24:E33" si="4">B24</f>
@@ -1983,17 +1966,17 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A25" s="90" t="s">
+      <c r="A25" s="88" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" s="89">
+        <v>0.5</v>
+      </c>
+      <c r="C25" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="90" t="s">
         <v>108</v>
-      </c>
-      <c r="B25" s="91">
-        <v>0.5</v>
-      </c>
-      <c r="C25" s="92" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="92" t="s">
-        <v>109</v>
       </c>
       <c r="E25" s="12">
         <f t="shared" si="4"/>
@@ -2001,17 +1984,17 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" s="93" t="s">
-        <v>107</v>
-      </c>
-      <c r="B26" s="94">
+      <c r="A26" s="91" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="92">
         <v>1</v>
       </c>
       <c r="C26" s="42" t="s">
         <v>7</v>
       </c>
       <c r="D26" s="54" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E26" s="13">
         <f t="shared" si="4"/>
@@ -2019,17 +2002,17 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A27" s="95" t="s">
-        <v>106</v>
-      </c>
-      <c r="B27" s="96">
-        <v>0</v>
-      </c>
-      <c r="C27" s="100" t="s">
+      <c r="A27" s="93" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="94">
+        <v>0</v>
+      </c>
+      <c r="C27" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="97" t="s">
-        <v>111</v>
+      <c r="D27" s="95" t="s">
+        <v>110</v>
       </c>
       <c r="E27" s="14">
         <f t="shared" si="4"/>
@@ -2037,17 +2020,17 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A28" s="98" t="s">
-        <v>105</v>
-      </c>
-      <c r="B28" s="94">
+      <c r="A28" s="96" t="s">
+        <v>104</v>
+      </c>
+      <c r="B28" s="92">
         <v>-0.5</v>
       </c>
-      <c r="C28" s="99" t="s">
+      <c r="C28" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="89" t="s">
-        <v>112</v>
+      <c r="D28" s="87" t="s">
+        <v>111</v>
       </c>
       <c r="E28" s="13">
         <f t="shared" si="4"/>
@@ -2055,17 +2038,17 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A29" s="93" t="s">
-        <v>104</v>
-      </c>
-      <c r="B29" s="94">
+      <c r="A29" s="91" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" s="92">
         <v>1</v>
       </c>
       <c r="C29" s="42" t="s">
         <v>7</v>
       </c>
       <c r="D29" s="54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E29" s="13">
         <f t="shared" si="4"/>
@@ -2073,17 +2056,17 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A30" s="95" t="s">
-        <v>103</v>
-      </c>
-      <c r="B30" s="96">
-        <v>0</v>
-      </c>
-      <c r="C30" s="97" t="s">
+      <c r="A30" s="93" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" s="94">
+        <v>0</v>
+      </c>
+      <c r="C30" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="97" t="s">
-        <v>114</v>
+      <c r="D30" s="95" t="s">
+        <v>113</v>
       </c>
       <c r="E30" s="14">
         <f t="shared" si="4"/>
@@ -2091,15 +2074,15 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A31" s="101" t="s">
+      <c r="A31" s="99" t="s">
+        <v>136</v>
+      </c>
+      <c r="B31" s="89">
+        <v>0</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="90" t="s">
         <v>139</v>
-      </c>
-      <c r="B31" s="91">
-        <v>0</v>
-      </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="92" t="s">
-        <v>142</v>
       </c>
       <c r="E31" s="12">
         <f t="shared" si="4"/>
@@ -2107,15 +2090,15 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A32" s="102" t="s">
-        <v>140</v>
-      </c>
-      <c r="B32" s="94">
+      <c r="A32" s="100" t="s">
+        <v>137</v>
+      </c>
+      <c r="B32" s="92">
         <v>-0.25</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="54" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E32" s="13">
         <f t="shared" si="4"/>
@@ -2123,15 +2106,15 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A33" s="103" t="s">
+      <c r="A33" s="101" t="s">
+        <v>138</v>
+      </c>
+      <c r="B33" s="94">
+        <v>0</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="95" t="s">
         <v>141</v>
-      </c>
-      <c r="B33" s="96">
-        <v>0</v>
-      </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="97" t="s">
-        <v>144</v>
       </c>
       <c r="E33" s="14">
         <f t="shared" si="4"/>
@@ -2139,17 +2122,17 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A34" s="104" t="s">
-        <v>84</v>
+      <c r="A34" s="102" t="s">
+        <v>83</v>
       </c>
       <c r="B34" s="2">
         <v>9.81</v>
       </c>
       <c r="C34" s="58" t="s">
+        <v>130</v>
+      </c>
+      <c r="D34" s="59" t="s">
         <v>131</v>
-      </c>
-      <c r="D34" s="59" t="s">
-        <v>132</v>
       </c>
       <c r="E34" s="1">
         <f>B34</f>
@@ -2157,11 +2140,11 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A35" s="101" t="s">
-        <v>167</v>
-      </c>
-      <c r="B35" s="91">
-        <v>1E-3</v>
+      <c r="A35" s="99" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" s="89">
+        <v>0.01</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>5</v>
@@ -2169,39 +2152,39 @@
       <c r="D35" s="4"/>
       <c r="E35" s="12">
         <f>B35</f>
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A36" s="102" t="s">
-        <v>168</v>
-      </c>
-      <c r="B36" s="94">
-        <v>1E-3</v>
+      <c r="A36" s="100" t="s">
+        <v>164</v>
+      </c>
+      <c r="B36" s="92">
+        <v>0.01</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="13">
         <f>B36</f>
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A37" s="103" t="s">
-        <v>169</v>
-      </c>
-      <c r="B37" s="96">
-        <v>1E-3</v>
+      <c r="A37" s="101" t="s">
+        <v>165</v>
+      </c>
+      <c r="B37" s="94">
+        <v>0.01</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="14">
         <f>B37</f>
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>
@@ -2258,7 +2241,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5">
         <v>24</v>
@@ -2299,12 +2282,12 @@
         <v>1</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B2" s="26">
         <v>0</v>
@@ -2313,7 +2296,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E2" s="29">
         <f>B2</f>
@@ -2322,7 +2305,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B3" s="20">
         <v>0</v>
@@ -2331,7 +2314,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E3" s="29">
         <f t="shared" ref="E3:E4" si="0">B3</f>
@@ -2340,13 +2323,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="55" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B4" s="56">
         <v>5</v>
       </c>
       <c r="C4" s="57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="31"/>
       <c r="E4" s="32">
@@ -2356,13 +2339,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="55" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B5" s="56">
         <v>0</v>
       </c>
       <c r="C5" s="57" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="29">
@@ -2372,13 +2355,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="56">
         <v>0</v>
       </c>
       <c r="C6" s="57" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="29">
@@ -2388,16 +2371,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="26">
         <v>0</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E7" s="29">
         <f t="shared" ref="E7" si="1">B7</f>
@@ -2406,16 +2389,16 @@
     </row>
     <row r="8" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" s="61">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E8" s="12">
         <f>B8</f>
@@ -2424,16 +2407,16 @@
     </row>
     <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="53" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B9" s="60">
         <v>0</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E9" s="12">
         <f t="shared" ref="E9" si="2">B9</f>
@@ -2442,7 +2425,7 @@
     </row>
     <row r="10" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10" s="62">
         <v>0</v>
@@ -2451,7 +2434,7 @@
         <v>23</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E10" s="50">
         <f>RADIANS(B10)/hr2sec</f>
@@ -2460,7 +2443,7 @@
     </row>
     <row r="11" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B11" s="61">
         <v>0</v>
@@ -2469,7 +2452,7 @@
         <v>23</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E11" s="50">
         <f>RADIANS(B11)/hr2sec</f>
@@ -2478,7 +2461,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B12" s="60">
         <v>0</v>
@@ -2487,7 +2470,7 @@
         <v>23</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E12" s="50">
         <f>RADIANS(B12)/hr2sec</f>
@@ -2496,7 +2479,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="62">
         <v>0</v>
@@ -2505,7 +2488,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E13" s="63">
         <f>B13</f>
@@ -2514,7 +2497,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="61">
         <v>20</v>
@@ -2523,7 +2506,7 @@
         <v>7</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E14" s="63">
         <f t="shared" ref="E14:E15" si="3">B14</f>
@@ -2532,7 +2515,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="60">
         <v>-0.15</v>
@@ -2541,7 +2524,7 @@
         <v>7</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E15" s="63">
         <f t="shared" si="3"/>
@@ -2635,12 +2618,12 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="4">
         <v>0.1</v>
@@ -2650,7 +2633,7 @@
         <v>m</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" s="50">
         <f t="shared" ref="E2:E7" si="0">B2</f>
@@ -2660,7 +2643,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="6">
         <v>0.2</v>
@@ -2670,7 +2653,7 @@
         <v>m</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E3" s="38">
         <f t="shared" si="0"/>
@@ -2680,7 +2663,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="6">
         <v>0.3</v>
@@ -2689,7 +2672,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E4" s="38">
         <f t="shared" si="0"/>
@@ -2699,16 +2682,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5" s="38">
         <f t="shared" si="0"/>
@@ -2718,16 +2701,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="6">
         <v>2</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E6" s="38">
         <f t="shared" si="0"/>
@@ -2737,7 +2720,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="6">
         <v>3</v>
@@ -2747,7 +2730,7 @@
         <v>m/sec</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E7" s="38">
         <f t="shared" si="0"/>
@@ -2757,7 +2740,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B8" s="6">
         <v>0.01</v>
@@ -2766,7 +2749,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8" s="38">
         <f>B8</f>
@@ -2776,7 +2759,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B9" s="6">
         <v>0.02</v>
@@ -2785,7 +2768,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="38">
         <f t="shared" ref="E9:E10" si="1">B9</f>
@@ -2795,7 +2778,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B10" s="6">
         <v>0.03</v>
@@ -2804,7 +2787,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E10" s="38">
         <f t="shared" si="1"/>
@@ -2814,16 +2797,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" s="16">
         <v>1E-3</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E11" s="38">
         <f>B11*g2mps2</f>
@@ -2833,16 +2816,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12" s="16">
         <v>2E-3</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E12" s="38">
         <f>B12*g2mps2</f>
@@ -2852,16 +2835,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="16">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E13" s="38">
         <f>B13*g2mps2</f>
@@ -2926,7 +2909,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" s="6">
         <v>0.11</v>
@@ -2935,7 +2918,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E17" s="38">
         <f t="shared" ref="E17:E19" si="2">B17</f>
@@ -2944,7 +2927,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" s="6">
         <v>0.22</v>
@@ -2953,7 +2936,7 @@
         <v>7</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E18" s="38">
         <f t="shared" si="2"/>
@@ -2962,7 +2945,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" s="8">
         <v>0.33</v>
@@ -2971,7 +2954,7 @@
         <v>7</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E19" s="39">
         <f t="shared" si="2"/>
@@ -3018,7 +3001,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -3035,7 +3018,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B3" s="6">
         <v>2</v>
@@ -3052,7 +3035,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B4" s="6">
         <v>3</v>
@@ -3069,7 +3052,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B5" s="16">
         <v>4</v>
@@ -3086,7 +3069,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="8">
         <v>5</v>
@@ -3103,7 +3086,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="6">
         <v>6</v>
@@ -3120,7 +3103,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="6">
         <v>9</v>
@@ -3137,7 +3120,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" s="6">
         <v>12</v>
@@ -3154,7 +3137,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" s="4">
         <f>B2</f>
@@ -3174,7 +3157,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="8">
         <f>B7</f>
@@ -3283,7 +3266,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="4">
         <v>11</v>
@@ -3300,7 +3283,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="6">
         <v>14</v>
@@ -3317,7 +3300,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="8">
         <v>17</v>
@@ -3334,7 +3317,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="6">
         <f>B2</f>
@@ -3355,7 +3338,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="8">
         <f>B5</f>
@@ -3384,7 +3367,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3411,21 +3394,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B2" s="25">
         <v>1E-3</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E2" s="11">
         <f>B2*g2mps2/3</f>
@@ -3434,18 +3417,18 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B3" s="10">
         <v>0.06</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="E3" s="108">
+        <v>154</v>
+      </c>
+      <c r="E3" s="106">
         <f>B3/SQRT(hr2sec)/3</f>
         <v>3.3333333333333332E-4</v>
       </c>
@@ -3482,23 +3465,23 @@
       <c r="D5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="108">
+      <c r="E5" s="106">
         <f>RADIANS(B5)/SQRT(hr2sec)/3</f>
         <v>4.8481368110953598E-6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B6" s="10">
         <v>1</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E6" s="11">
         <f>B6/3</f>
@@ -3507,7 +3490,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B7" s="10">
         <v>1</v>
@@ -3516,7 +3499,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E7" s="11">
         <f>B7/3</f>
@@ -3525,7 +3508,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B8" s="10">
         <v>1</v>
@@ -3534,7 +3517,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E8" s="11">
         <f>B8/3</f>
@@ -3543,20 +3526,20 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="16" t="s">
-        <v>161</v>
+        <v>195</v>
       </c>
       <c r="B9" s="10">
-        <v>9.9999999999999995E-7</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E9" s="11">
         <f>B9/3</f>
-        <v>3.333333333333333E-7</v>
+        <v>3.3333333333333337E-6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -3626,12 +3609,12 @@
         <v>1</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -3640,7 +3623,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E2" s="12">
         <f t="shared" ref="E2:E4" si="0">B2/3</f>
@@ -3649,7 +3632,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B3" s="8">
         <v>1</v>
@@ -3658,7 +3641,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E3" s="14">
         <f t="shared" si="0"/>
@@ -3667,70 +3650,70 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="55" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B4" s="57">
         <v>0.1</v>
       </c>
       <c r="C4" s="57" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="57" t="s">
-        <v>171</v>
-      </c>
-      <c r="E4" s="105">
+        <v>167</v>
+      </c>
+      <c r="E4" s="103">
         <f t="shared" si="0"/>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="55" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B5" s="57">
         <v>1</v>
       </c>
       <c r="C5" s="57" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D5" s="57" t="s">
-        <v>176</v>
-      </c>
-      <c r="E5" s="105">
+        <v>172</v>
+      </c>
+      <c r="E5" s="103">
         <f>RADIANS(B5)/3</f>
         <v>5.8177641733144318E-3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="55" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B6" s="57">
         <v>1</v>
       </c>
       <c r="C6" s="57" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D6" s="57" t="s">
-        <v>177</v>
-      </c>
-      <c r="E6" s="105">
+        <v>173</v>
+      </c>
+      <c r="E6" s="103">
         <f>RADIANS(B6)/3</f>
         <v>5.8177641733144318E-3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B7" s="4">
         <v>1E-3</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E7" s="12">
         <f>B7*g2mps2/3</f>
@@ -3739,16 +3722,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B8" s="6">
         <v>1E-3</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E8" s="13">
         <f>B8*g2mps2/3</f>
@@ -3757,16 +3740,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="19" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B9" s="8">
         <v>1E-3</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E9" s="14">
         <f>B9*g2mps2/3</f>
@@ -3774,8 +3757,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="106" t="s">
-        <v>183</v>
+      <c r="A10" s="104" t="s">
+        <v>179</v>
       </c>
       <c r="B10" s="4">
         <v>5</v>
@@ -3784,7 +3767,7 @@
         <v>23</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" s="12">
         <f>RADIANS(B10)/hr2sec/3</f>
@@ -3793,7 +3776,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="18" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B11" s="6">
         <v>5</v>
@@ -3802,7 +3785,7 @@
         <v>23</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" s="13">
         <f>RADIANS(B11)/hr2sec/3</f>
@@ -3811,7 +3794,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="19" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B12" s="8">
         <v>5</v>
@@ -3820,7 +3803,7 @@
         <v>23</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12" s="14">
         <f>RADIANS(B12)/hr2sec/3</f>
@@ -3828,8 +3811,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="106" t="s">
-        <v>186</v>
+      <c r="A13" s="104" t="s">
+        <v>182</v>
       </c>
       <c r="B13" s="4">
         <v>1E-3</v>
@@ -3837,8 +3820,8 @@
       <c r="C13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="107" t="s">
-        <v>190</v>
+      <c r="D13" s="105" t="s">
+        <v>186</v>
       </c>
       <c r="E13" s="12">
         <f>B13/3</f>
@@ -3847,7 +3830,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B14" s="6">
         <v>1E-3</v>
@@ -3856,7 +3839,7 @@
         <v>7</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E14" s="13">
         <f t="shared" ref="E14:E15" si="1">B14/3</f>
@@ -3865,7 +3848,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B15" s="8">
         <v>1E-3</v>
@@ -3874,7 +3857,7 @@
         <v>7</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E15" s="14">
         <f t="shared" si="1"/>
@@ -3892,7 +3875,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3919,22 +3902,22 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B2" s="83">
+        <v>150</v>
+      </c>
+      <c r="B2" s="81">
         <f>truthStateParams!B2</f>
         <v>1E-3</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E2" s="11">
         <f>B2*g2mps2/3</f>
@@ -3943,19 +3926,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B3" s="83">
+        <v>152</v>
+      </c>
+      <c r="B3" s="81">
         <f>truthStateParams!B3</f>
         <v>0.06</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="E3" s="108">
+        <v>154</v>
+      </c>
+      <c r="E3" s="106">
         <f>B3/SQRT(hr2sec)/3</f>
         <v>3.3333333333333332E-4</v>
       </c>
@@ -3965,7 +3948,7 @@
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="83">
+      <c r="B4" s="81">
         <f>truthStateParams!B4</f>
         <v>5</v>
       </c>
@@ -3984,7 +3967,7 @@
       <c r="A5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="83">
+      <c r="B5" s="81">
         <f>truthStateParams!B5</f>
         <v>0.05</v>
       </c>
@@ -3994,24 +3977,24 @@
       <c r="D5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="108">
+      <c r="E5" s="106">
         <f>RADIANS(B5)/SQRT(hr2sec)/3</f>
         <v>4.8481368110953598E-6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="B6" s="83">
+        <v>155</v>
+      </c>
+      <c r="B6" s="81">
         <f>truthStateParams!B6</f>
         <v>1</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E6" s="11">
         <f>B6/3</f>
@@ -4020,9 +4003,9 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="B7" s="83">
+        <v>156</v>
+      </c>
+      <c r="B7" s="81">
         <f>truthStateParams!B7</f>
         <v>1</v>
       </c>
@@ -4030,7 +4013,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E7" s="11">
         <f>B7/3</f>
@@ -4039,9 +4022,9 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="B8" s="83">
+        <v>157</v>
+      </c>
+      <c r="B8" s="81">
         <f>truthStateParams!B8</f>
         <v>1</v>
       </c>
@@ -4049,7 +4032,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E8" s="11">
         <f>B8/3</f>
@@ -4058,19 +4041,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="B9" s="83">
+        <v>195</v>
+      </c>
+      <c r="B9" s="81">
         <f>truthStateParams!B9</f>
-        <v>9.9999999999999995E-7</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="11">
         <f>B9/3</f>
-        <v>3.333333333333333E-7</v>
+        <v>3.3333333333333337E-6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -4112,7 +4095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -4140,7 +4123,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -4191,7 +4174,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B4" s="8">
         <v>1E-3</v>
@@ -4200,7 +4183,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E4" s="39">
         <f t="shared" si="0"/>
@@ -4210,7 +4193,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B5" s="4">
         <f>truthStateInitialUncertainty!B4</f>
@@ -4232,7 +4215,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B6" s="6">
         <f>truthStateInitialUncertainty!B4</f>
@@ -4253,7 +4236,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B7" s="8">
         <f>truthStateInitialUncertainty!B4</f>
@@ -4274,7 +4257,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B8" s="4">
         <v>1E-3</v>
@@ -4284,7 +4267,7 @@
         <v xml:space="preserve">deg </v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E8" s="50">
         <f t="shared" ref="E8:E9" si="1">RADIANS(B8)/3</f>
@@ -4293,7 +4276,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B9" s="6">
         <v>1E-3</v>
@@ -4303,7 +4286,7 @@
         <v xml:space="preserve">deg </v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E9" s="38">
         <f t="shared" si="1"/>
@@ -4312,7 +4295,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="7" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B10" s="8">
         <f>truthStateInitialUncertainty!B6</f>
@@ -4323,7 +4306,7 @@
         <v xml:space="preserve">deg </v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E10" s="39">
         <f>RADIANS(B10)/3</f>

</xml_diff>

<commit_message>
fixed errors in Monte Carlo with addition of discrete measurements, documented results
</commit_message>
<xml_diff>
--- a/MATLAB Code/config.xlsx
+++ b/MATLAB Code/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ikeni\Desktop\Optimal Estimation\USU_Optimal_Estimation_Project\MATLAB Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5A09AF-B543-41D0-93E3-4CEBC1111CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D7742F-4EC3-4ED9-A4C5-1127C242DF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="3540" windowWidth="15390" windowHeight="9540" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="198">
   <si>
     <t>Value</t>
   </si>
@@ -638,18 +638,6 @@
   </si>
   <si>
     <t>3-sigma pdoa measurement noise</t>
-  </si>
-  <si>
-    <t>processNoiseOn</t>
-  </si>
-  <si>
-    <t>measurementNoiseOn</t>
-  </si>
-  <si>
-    <t>flag to enable synthesis of measurement noise</t>
-  </si>
-  <si>
-    <t>flag to enable synthesis of process noise</t>
   </si>
   <si>
     <t>measLinearizationCheckEnable</t>
@@ -1070,7 +1058,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1178,8 +1166,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1518,10 +1504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1664,7 +1650,7 @@
         <v>57</v>
       </c>
       <c r="B8" s="77">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="C8" s="42" t="s">
         <v>4</v>
@@ -1674,7 +1660,7 @@
       </c>
       <c r="E8" s="44">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.45">
@@ -1691,7 +1677,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="44">
-        <f t="shared" ref="E9:E22" si="1">B9</f>
+        <f t="shared" ref="E9:E20" si="1">B9</f>
         <v>0</v>
       </c>
     </row>
@@ -1715,7 +1701,7 @@
     </row>
     <row r="11" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="74" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B11" s="75">
         <v>0</v>
@@ -1754,7 +1740,7 @@
         <v>132</v>
       </c>
       <c r="B13" s="73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="66" t="s">
         <v>4</v>
@@ -1764,7 +1750,7 @@
       </c>
       <c r="E13" s="64">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.45">
@@ -1835,355 +1821,319 @@
         <v>147</v>
       </c>
       <c r="E17" s="64">
-        <f t="shared" ref="E17:E19" si="3">B17</f>
+        <f t="shared" ref="E17" si="3">B17</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A18" s="72" t="s">
-        <v>198</v>
-      </c>
-      <c r="B18" s="73">
-        <v>1</v>
-      </c>
-      <c r="C18" s="66" t="s">
-        <v>4</v>
+      <c r="A18" s="67" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2</v>
+      </c>
+      <c r="C18" s="42" t="s">
+        <v>91</v>
       </c>
       <c r="D18" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="E18" s="64">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A19" s="107" t="s">
-        <v>197</v>
-      </c>
-      <c r="B19" s="108">
-        <v>1</v>
-      </c>
-      <c r="C19" s="66" t="s">
-        <v>4</v>
+      <c r="A19" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="2">
+        <v>100</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>5</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>200</v>
-      </c>
-      <c r="E19" s="64">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>95</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="1"/>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A20" s="67" t="s">
-        <v>90</v>
+      <c r="A20" s="42" t="s">
+        <v>94</v>
       </c>
       <c r="B20" s="2">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="C20" s="42" t="s">
-        <v>91</v>
+        <v>5</v>
       </c>
       <c r="D20" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="42" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B21" s="2">
+        <v>122</v>
+      </c>
+      <c r="C21" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="1">
+        <f>B21*1000000</f>
+        <v>122000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" s="76" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="E21" s="1">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A22" s="42" t="s">
-        <v>94</v>
-      </c>
       <c r="B22" s="2">
-        <v>100</v>
-      </c>
-      <c r="C22" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="42" t="s">
-        <v>96</v>
+        <v>299702547</v>
+      </c>
+      <c r="C22" s="76" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="76" t="s">
+        <v>101</v>
       </c>
       <c r="E22" s="1">
-        <f t="shared" si="1"/>
-        <v>100</v>
+        <f t="shared" ref="E22:E31" si="4">B22</f>
+        <v>299702547</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A23" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="B23" s="2">
-        <v>122</v>
-      </c>
-      <c r="C23" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="D23" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="E23" s="1">
-        <f>B23*1000000</f>
-        <v>122000000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A24" s="76" t="s">
-        <v>100</v>
-      </c>
-      <c r="B24" s="2">
-        <v>299702547</v>
-      </c>
-      <c r="C24" s="76" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="76" t="s">
-        <v>101</v>
-      </c>
-      <c r="E24" s="1">
-        <f t="shared" ref="E24:E33" si="4">B24</f>
-        <v>299702547</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A25" s="88" t="s">
+      <c r="A23" s="88" t="s">
         <v>107</v>
       </c>
-      <c r="B25" s="89">
+      <c r="B23" s="89">
         <v>0.5</v>
       </c>
-      <c r="C25" s="90" t="s">
+      <c r="C23" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="90" t="s">
+      <c r="D23" s="90" t="s">
         <v>108</v>
       </c>
-      <c r="E25" s="12">
+      <c r="E23" s="12">
         <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
     </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" s="91" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="92">
+        <v>1</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="E24" s="13">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" s="93" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" s="94">
+        <v>0</v>
+      </c>
+      <c r="C25" s="98" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="95" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" s="91" t="s">
-        <v>106</v>
+      <c r="A26" s="96" t="s">
+        <v>104</v>
       </c>
       <c r="B26" s="92">
-        <v>1</v>
-      </c>
-      <c r="C26" s="42" t="s">
+        <v>-0.5</v>
+      </c>
+      <c r="C26" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="54" t="s">
-        <v>109</v>
+      <c r="D26" s="87" t="s">
+        <v>111</v>
       </c>
       <c r="E26" s="13">
         <f t="shared" si="4"/>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" s="91" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="92">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A27" s="93" t="s">
-        <v>105</v>
-      </c>
-      <c r="B27" s="94">
-        <v>0</v>
-      </c>
-      <c r="C27" s="98" t="s">
+      <c r="C27" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="95" t="s">
-        <v>110</v>
-      </c>
-      <c r="E27" s="14">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A28" s="96" t="s">
-        <v>104</v>
-      </c>
-      <c r="B28" s="92">
-        <v>-0.5</v>
-      </c>
-      <c r="C28" s="97" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="87" t="s">
-        <v>111</v>
-      </c>
-      <c r="E28" s="13">
-        <f t="shared" si="4"/>
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A29" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="B29" s="92">
-        <v>1</v>
-      </c>
-      <c r="C29" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="54" t="s">
+      <c r="D27" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E27" s="13">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28" s="93" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="94">
+        <v>0</v>
+      </c>
+      <c r="C28" s="95" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="95" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29" s="99" t="s">
+        <v>136</v>
+      </c>
+      <c r="B29" s="89">
+        <v>0</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="90" t="s">
+        <v>139</v>
+      </c>
+      <c r="E29" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A30" s="93" t="s">
-        <v>102</v>
-      </c>
-      <c r="B30" s="94">
-        <v>0</v>
-      </c>
-      <c r="C30" s="95" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="95" t="s">
-        <v>113</v>
-      </c>
-      <c r="E30" s="14">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A31" s="99" t="s">
-        <v>136</v>
-      </c>
-      <c r="B31" s="89">
-        <v>0</v>
-      </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="90" t="s">
-        <v>139</v>
-      </c>
-      <c r="E31" s="12">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A32" s="100" t="s">
+      <c r="A30" s="100" t="s">
         <v>137</v>
       </c>
-      <c r="B32" s="92">
+      <c r="B30" s="92">
         <v>-0.25</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="54" t="s">
+      <c r="C30" s="6"/>
+      <c r="D30" s="54" t="s">
         <v>140</v>
       </c>
-      <c r="E32" s="13">
+      <c r="E30" s="13">
         <f t="shared" si="4"/>
         <v>-0.25</v>
       </c>
     </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31" s="101" t="s">
+        <v>138</v>
+      </c>
+      <c r="B31" s="94">
+        <v>0</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="95" t="s">
+        <v>141</v>
+      </c>
+      <c r="E31" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32" s="102" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" s="2">
+        <v>9.81</v>
+      </c>
+      <c r="C32" s="58" t="s">
+        <v>130</v>
+      </c>
+      <c r="D32" s="59" t="s">
+        <v>131</v>
+      </c>
+      <c r="E32" s="1">
+        <f>B32</f>
+        <v>9.81</v>
+      </c>
+    </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A33" s="101" t="s">
-        <v>138</v>
-      </c>
-      <c r="B33" s="94">
-        <v>0</v>
-      </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="95" t="s">
-        <v>141</v>
-      </c>
-      <c r="E33" s="14">
-        <f t="shared" si="4"/>
-        <v>0</v>
+      <c r="A33" s="99" t="s">
+        <v>163</v>
+      </c>
+      <c r="B33" s="89">
+        <v>0.01</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="12">
+        <f>B33</f>
+        <v>0.01</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A34" s="102" t="s">
-        <v>83</v>
-      </c>
-      <c r="B34" s="2">
-        <v>9.81</v>
-      </c>
-      <c r="C34" s="58" t="s">
-        <v>130</v>
-      </c>
-      <c r="D34" s="59" t="s">
-        <v>131</v>
-      </c>
-      <c r="E34" s="1">
+      <c r="A34" s="100" t="s">
+        <v>164</v>
+      </c>
+      <c r="B34" s="92">
+        <v>0.01</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D34" s="6"/>
+      <c r="E34" s="13">
         <f>B34</f>
-        <v>9.81</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A35" s="99" t="s">
-        <v>163</v>
-      </c>
-      <c r="B35" s="89">
+      <c r="A35" s="101" t="s">
+        <v>165</v>
+      </c>
+      <c r="B35" s="94">
         <v>0.01</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="12">
+      <c r="C35" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D35" s="8"/>
+      <c r="E35" s="14">
         <f>B35</f>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A36" s="100" t="s">
-        <v>164</v>
-      </c>
-      <c r="B36" s="92">
-        <v>0.01</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="13">
-        <f>B36</f>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A37" s="101" t="s">
-        <v>165</v>
-      </c>
-      <c r="B37" s="94">
-        <v>0.01</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="14">
-        <f>B37</f>
         <v>0.01</v>
       </c>
     </row>
@@ -3367,7 +3317,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>